<commit_message>
updated excel tables to match intended SQL table design
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syntel.MININT-1GOAKQE\Documents\Git\CaseStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
-  <si>
-    <t>Item Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>fries</t>
   </si>
@@ -50,138 +44,42 @@
     <t>price</t>
   </si>
   <si>
-    <t>Item ID</t>
-  </si>
-  <si>
-    <t>Order ID</t>
-  </si>
-  <si>
     <t>Order Details</t>
   </si>
   <si>
     <t>Menu Items</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Location_ID</t>
-  </si>
-  <si>
     <t>Locations</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>ZIP</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Vegetarian</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Photo</t>
-  </si>
-  <si>
     <t>Users</t>
   </si>
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>User_ID</t>
-  </si>
-  <si>
-    <t>Passwords</t>
-  </si>
-  <si>
-    <t>Placed Time</t>
-  </si>
-  <si>
-    <t>Placed Date</t>
-  </si>
-  <si>
-    <t>Delivery Date</t>
-  </si>
-  <si>
-    <t>Delivery Time</t>
-  </si>
-  <si>
     <t>Verified</t>
   </si>
   <si>
-    <t>Payment_ID</t>
-  </si>
-  <si>
-    <t>Card_Number</t>
-  </si>
-  <si>
-    <t>Security Code</t>
-  </si>
-  <si>
-    <t>Saved Payment Options</t>
-  </si>
-  <si>
-    <t>Expirey_Date</t>
-  </si>
-  <si>
-    <t>Doug Jones</t>
-  </si>
-  <si>
     <t>dougyj@hotmail.com</t>
   </si>
   <si>
     <t>(null if cash)</t>
   </si>
   <si>
-    <t>Status_ID</t>
-  </si>
-  <si>
-    <t>Status_Name</t>
-  </si>
-  <si>
     <t>Unverified</t>
   </si>
   <si>
     <t>BANNED</t>
   </si>
   <si>
-    <t>Freddy Bing</t>
-  </si>
-  <si>
     <t>bingboy@xxx.com</t>
   </si>
   <si>
     <t>Phoenix</t>
   </si>
   <si>
-    <t>Instructions</t>
-  </si>
-  <si>
-    <t>Slot_ID</t>
-  </si>
-  <si>
-    <t>Time_Start</t>
-  </si>
-  <si>
-    <t>Time_End</t>
-  </si>
-  <si>
-    <t>Time_Name</t>
-  </si>
-  <si>
     <t>Time Slots</t>
   </si>
   <si>
@@ -194,12 +92,6 @@
     <t>Breakfast</t>
   </si>
   <si>
-    <t>Combo_ID</t>
-  </si>
-  <si>
-    <t>Item_ID</t>
-  </si>
-  <si>
     <t>Combos</t>
   </si>
   <si>
@@ -209,39 +101,15 @@
     <t>Manager</t>
   </si>
   <si>
-    <t>Store_ID</t>
-  </si>
-  <si>
-    <t>Store_name</t>
-  </si>
-  <si>
-    <t>Open_time</t>
-  </si>
-  <si>
-    <t>Close_time</t>
-  </si>
-  <si>
     <t>Stores</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Manager_ID</t>
-  </si>
-  <si>
-    <t>Delivery_Method_ID</t>
-  </si>
-  <si>
     <t>Delivery Methods</t>
   </si>
   <si>
     <t>pickup</t>
   </si>
   <si>
-    <t>Delivery_Method_Description</t>
-  </si>
-  <si>
     <t>delivery</t>
   </si>
   <si>
@@ -251,9 +119,6 @@
     <t>Tables</t>
   </si>
   <si>
-    <t>Items in Orders</t>
-  </si>
-  <si>
     <t>items in Orders</t>
   </si>
   <si>
@@ -263,15 +128,6 @@
     <t>User Status</t>
   </si>
   <si>
-    <t>Delivery_Status_ID</t>
-  </si>
-  <si>
-    <t>Delivery_Status_Description</t>
-  </si>
-  <si>
-    <t>Delivery statuses</t>
-  </si>
-  <si>
     <t>pending</t>
   </si>
   <si>
@@ -290,7 +146,190 @@
     <t>Specials</t>
   </si>
   <si>
-    <t>Discount Percentage</t>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>vegetarian</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>time_slot_id</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>specials</t>
+  </si>
+  <si>
+    <t>discount_percentage</t>
+  </si>
+  <si>
+    <t>combos</t>
+  </si>
+  <si>
+    <t>combo_id</t>
+  </si>
+  <si>
+    <t>time_slots</t>
+  </si>
+  <si>
+    <t>slot_end</t>
+  </si>
+  <si>
+    <t>slot_id</t>
+  </si>
+  <si>
+    <t>slot_start</t>
+  </si>
+  <si>
+    <t>slot_name</t>
+  </si>
+  <si>
+    <t>order_items</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>placed_timestamp</t>
+  </si>
+  <si>
+    <t>delivery_timestamp</t>
+  </si>
+  <si>
+    <t>payment_id</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>delivery_method_id</t>
+  </si>
+  <si>
+    <t>store_id</t>
+  </si>
+  <si>
+    <t>delivery_status_id</t>
+  </si>
+  <si>
+    <t>delivery_statuses</t>
+  </si>
+  <si>
+    <t>selivery_status_is</t>
+  </si>
+  <si>
+    <t>delivery_status</t>
+  </si>
+  <si>
+    <t>delivery_method</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Freddy</t>
+  </si>
+  <si>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>user_status_id</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>location_is</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>cards</t>
+  </si>
+  <si>
+    <t>card_id</t>
+  </si>
+  <si>
+    <t>card_number</t>
+  </si>
+  <si>
+    <t>expiry_date</t>
+  </si>
+  <si>
+    <t>security_code</t>
+  </si>
+  <si>
+    <t>user_statuses</t>
+  </si>
+  <si>
+    <t>user_status</t>
+  </si>
+  <si>
+    <t>stores</t>
+  </si>
+  <si>
+    <t>store</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>manager_id</t>
+  </si>
+  <si>
+    <t>open_time</t>
+  </si>
+  <si>
+    <t>close_time</t>
   </si>
 </sst>
 </file>
@@ -504,6 +543,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,10 +565,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -807,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BT16"/>
+  <dimension ref="A2:BS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="BM1" workbookViewId="0">
+      <selection activeCell="BS13" sqref="BS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,329 +857,325 @@
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.7109375" customWidth="1"/>
-    <col min="33" max="33" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.42578125" customWidth="1"/>
-    <col min="35" max="35" width="18" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.28515625" customWidth="1"/>
-    <col min="48" max="48" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="11" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11" customWidth="1"/>
+    <col min="44" max="44" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
-      <c r="K3" s="17" t="s">
+    <row r="2" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="K3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="N3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="Q3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="20"/>
+      <c r="V3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="20"/>
+      <c r="Y3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="20"/>
+      <c r="AI3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" s="23"/>
+      <c r="AL3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM3" s="23"/>
+      <c r="AO3" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="20"/>
+      <c r="AW3" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX3" s="19"/>
+      <c r="AY3" s="19"/>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="19"/>
+      <c r="BB3" s="20"/>
+      <c r="BD3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="BE3" s="19"/>
+      <c r="BF3" s="19"/>
+      <c r="BG3" s="19"/>
+      <c r="BH3" s="20"/>
+      <c r="BJ3" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="BK3" s="20"/>
+      <c r="BM3" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="BN3" s="22"/>
+      <c r="BO3" s="22"/>
+      <c r="BP3" s="22"/>
+      <c r="BQ3" s="22"/>
+      <c r="BR3" s="22"/>
+      <c r="BS3" s="23"/>
+    </row>
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ4" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AX4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="BA4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="N3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="16"/>
-      <c r="Q3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="16"/>
-      <c r="V3" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="W3" s="16"/>
-      <c r="Y3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="16"/>
-      <c r="AK3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL3" s="19"/>
-      <c r="AN3" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO3" s="19"/>
-      <c r="AQ3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR3" s="15"/>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15"/>
-      <c r="AV3" s="16"/>
-      <c r="AX3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AY3" s="15"/>
-      <c r="AZ3" s="15"/>
-      <c r="BA3" s="15"/>
-      <c r="BB3" s="15"/>
-      <c r="BC3" s="16"/>
-      <c r="BE3" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BF3" s="15"/>
-      <c r="BG3" s="15"/>
-      <c r="BH3" s="15"/>
-      <c r="BI3" s="16"/>
-      <c r="BK3" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="BL3" s="16"/>
-      <c r="BN3" s="17" t="s">
+      <c r="BB4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="BG4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="BH4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BM4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO3" s="18"/>
-      <c r="BP3" s="18"/>
-      <c r="BQ3" s="18"/>
-      <c r="BR3" s="18"/>
-      <c r="BS3" s="18"/>
-      <c r="BT3" s="19"/>
+      <c r="BN4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="BP4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="BQ4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="BR4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="BS4" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AR4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AU4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AY4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AZ4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="BA4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="BB4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="BC4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="BG4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="BH4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="BK4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BL4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="BN4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BO4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="BP4" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="BQ4" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="BR4" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="BS4" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="BT4" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>87</v>
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
@@ -1161,13 +1196,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="V5" s="3">
         <v>2</v>
@@ -1187,83 +1222,84 @@
         <v>1</v>
       </c>
       <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="4"/>
-      <c r="AK5" s="3">
+      <c r="AG5" s="4"/>
+      <c r="AI5" s="3">
         <v>0</v>
       </c>
-      <c r="AL5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN5" s="3">
+      <c r="AJ5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL5" s="3">
         <v>0</v>
       </c>
-      <c r="AO5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ5" s="3">
+      <c r="AM5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO5" s="3">
         <v>0</v>
       </c>
-      <c r="AR5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AS5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AT5" s="7"/>
-      <c r="AU5" s="7">
+      <c r="AP5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS5" s="7"/>
+      <c r="AT5" s="7">
         <v>1</v>
       </c>
-      <c r="AV5" s="4"/>
-      <c r="AX5" s="3">
+      <c r="AU5" s="4"/>
+      <c r="AW5" s="3">
         <v>0</v>
       </c>
+      <c r="AX5" s="7"/>
       <c r="AY5" s="7"/>
-      <c r="AZ5" s="7"/>
-      <c r="BA5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="BB5" s="7"/>
-      <c r="BC5" s="4"/>
-      <c r="BE5" s="3">
+      <c r="AZ5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA5" s="7"/>
+      <c r="BB5" s="4"/>
+      <c r="BD5" s="3">
         <v>0</v>
       </c>
-      <c r="BF5" s="7">
+      <c r="BE5" s="7">
         <v>1</v>
       </c>
-      <c r="BG5" s="10">
+      <c r="BF5" s="10">
         <v>554466778899</v>
       </c>
-      <c r="BH5" s="12">
+      <c r="BG5" s="12">
         <v>43718</v>
       </c>
-      <c r="BI5" s="4">
+      <c r="BH5" s="4">
         <v>234</v>
       </c>
-      <c r="BK5" s="3">
+      <c r="BJ5" s="3">
         <v>0</v>
       </c>
-      <c r="BL5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="BN5" s="3"/>
+      <c r="BK5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM5" s="3"/>
+      <c r="BN5" s="7"/>
       <c r="BO5" s="7"/>
       <c r="BP5" s="7"/>
       <c r="BQ5" s="7"/>
       <c r="BR5" s="7"/>
-      <c r="BS5" s="7"/>
-      <c r="BT5" s="4"/>
+      <c r="BS5" s="4"/>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>58</v>
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
@@ -1302,81 +1338,82 @@
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
-      <c r="AG6" s="7"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="4"/>
-      <c r="AK6" s="3">
+      <c r="AG6" s="4"/>
+      <c r="AI6" s="3">
         <v>1</v>
       </c>
-      <c r="AL6" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN6" s="3">
+      <c r="AJ6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL6" s="3">
         <v>1</v>
       </c>
-      <c r="AO6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ6" s="3">
+      <c r="AM6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO6" s="3">
         <v>1</v>
       </c>
-      <c r="AR6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT6" s="7"/>
-      <c r="AU6" s="7">
+      <c r="AP6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS6" s="7"/>
+      <c r="AT6" s="7">
         <v>0</v>
       </c>
-      <c r="AV6" s="4"/>
-      <c r="AX6" s="3">
+      <c r="AU6" s="4"/>
+      <c r="AW6" s="3">
         <v>1</v>
       </c>
+      <c r="AX6" s="7"/>
       <c r="AY6" s="7"/>
       <c r="AZ6" s="7"/>
       <c r="BA6" s="7"/>
-      <c r="BB6" s="7"/>
-      <c r="BC6" s="4"/>
-      <c r="BE6" s="3">
+      <c r="BB6" s="4"/>
+      <c r="BD6" s="3">
         <v>1</v>
       </c>
-      <c r="BF6" s="7">
+      <c r="BE6" s="7">
         <v>1</v>
       </c>
-      <c r="BG6" s="10">
+      <c r="BF6" s="10">
         <v>683967034588</v>
       </c>
-      <c r="BH6" s="12">
+      <c r="BG6" s="12">
         <v>43957</v>
       </c>
-      <c r="BI6" s="4">
+      <c r="BH6" s="4">
         <v>354</v>
       </c>
-      <c r="BK6" s="3">
+      <c r="BJ6" s="3">
         <v>1</v>
       </c>
-      <c r="BL6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="BN6" s="3"/>
+      <c r="BK6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BM6" s="3"/>
+      <c r="BN6" s="7"/>
       <c r="BO6" s="7"/>
       <c r="BP6" s="7"/>
       <c r="BQ6" s="7"/>
       <c r="BR6" s="7"/>
-      <c r="BS6" s="7"/>
-      <c r="BT6" s="4"/>
+      <c r="BS6" s="4"/>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>52</v>
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" s="7">
         <v>0</v>
@@ -1415,75 +1452,74 @@
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="4"/>
-      <c r="AK7" s="3">
+      <c r="AG7" s="4"/>
+      <c r="AI7" s="3">
         <v>2</v>
       </c>
-      <c r="AL7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AN7" s="3">
+      <c r="AJ7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL7" s="3">
         <v>2</v>
       </c>
-      <c r="AO7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ7" s="3">
+      <c r="AM7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO7" s="3">
         <v>2</v>
       </c>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
       <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
       <c r="AT7" s="7"/>
-      <c r="AU7" s="7"/>
-      <c r="AV7" s="4"/>
-      <c r="AX7" s="3">
+      <c r="AU7" s="4"/>
+      <c r="AW7" s="3">
         <v>2</v>
       </c>
+      <c r="AX7" s="7"/>
       <c r="AY7" s="7"/>
       <c r="AZ7" s="7"/>
       <c r="BA7" s="7"/>
-      <c r="BB7" s="7"/>
-      <c r="BC7" s="4"/>
-      <c r="BE7" s="3">
+      <c r="BB7" s="4"/>
+      <c r="BD7" s="3">
         <v>2</v>
       </c>
-      <c r="BF7" s="7">
+      <c r="BE7" s="7">
         <v>2</v>
       </c>
-      <c r="BG7" s="10">
+      <c r="BF7" s="10">
         <v>338744976569</v>
       </c>
-      <c r="BH7" s="12">
+      <c r="BG7" s="12">
         <v>45770</v>
       </c>
-      <c r="BI7" s="4">
+      <c r="BH7" s="4">
         <v>325</v>
       </c>
-      <c r="BK7" s="3">
+      <c r="BJ7" s="3">
         <v>2</v>
       </c>
-      <c r="BL7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="BN7" s="3"/>
+      <c r="BK7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="BM7" s="3"/>
+      <c r="BN7" s="7"/>
       <c r="BO7" s="7"/>
       <c r="BP7" s="7"/>
       <c r="BQ7" s="7"/>
       <c r="BR7" s="7"/>
-      <c r="BS7" s="7"/>
-      <c r="BT7" s="4"/>
+      <c r="BS7" s="4"/>
     </row>
-    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>76</v>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="3">
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1520,63 +1556,62 @@
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="7"/>
-      <c r="AG8" s="7"/>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="4"/>
-      <c r="AK8" s="3">
+      <c r="AG8" s="4"/>
+      <c r="AI8" s="3">
         <v>3</v>
       </c>
-      <c r="AL8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="4"/>
-      <c r="AQ8" s="3">
+      <c r="AJ8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="4"/>
+      <c r="AO8" s="3">
         <v>3</v>
       </c>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
       <c r="AR8" s="7"/>
       <c r="AS8" s="7"/>
       <c r="AT8" s="7"/>
-      <c r="AU8" s="7"/>
-      <c r="AV8" s="4"/>
-      <c r="AX8" s="3">
+      <c r="AU8" s="4"/>
+      <c r="AW8" s="3">
         <v>3</v>
       </c>
+      <c r="AX8" s="7"/>
       <c r="AY8" s="7"/>
       <c r="AZ8" s="7"/>
       <c r="BA8" s="7"/>
-      <c r="BB8" s="7"/>
-      <c r="BC8" s="4"/>
-      <c r="BE8" s="3">
+      <c r="BB8" s="4"/>
+      <c r="BD8" s="3">
         <v>3</v>
       </c>
-      <c r="BF8" s="7"/>
-      <c r="BG8" s="10"/>
-      <c r="BH8" s="7"/>
-      <c r="BI8" s="4"/>
-      <c r="BK8" s="3">
+      <c r="BE8" s="7"/>
+      <c r="BF8" s="10"/>
+      <c r="BG8" s="7"/>
+      <c r="BH8" s="4"/>
+      <c r="BJ8" s="3">
         <v>3</v>
       </c>
-      <c r="BL8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BN8" s="3"/>
+      <c r="BK8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="BM8" s="3"/>
+      <c r="BN8" s="7"/>
       <c r="BO8" s="7"/>
       <c r="BP8" s="7"/>
       <c r="BQ8" s="7"/>
       <c r="BR8" s="7"/>
-      <c r="BS8" s="7"/>
-      <c r="BT8" s="4"/>
+      <c r="BS8" s="4"/>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>10</v>
+    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="C9" s="3">
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1609,53 +1644,52 @@
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
-      <c r="AG9" s="7"/>
-      <c r="AH9" s="7"/>
-      <c r="AI9" s="4"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="4"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="4"/>
-      <c r="AQ9" s="3">
+      <c r="AG9" s="4"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="4"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="4"/>
+      <c r="AO9" s="3">
         <v>4</v>
       </c>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
       <c r="AR9" s="7"/>
       <c r="AS9" s="7"/>
       <c r="AT9" s="7"/>
-      <c r="AU9" s="7"/>
-      <c r="AV9" s="4"/>
-      <c r="AX9" s="3">
+      <c r="AU9" s="4"/>
+      <c r="AW9" s="3">
         <v>4</v>
       </c>
+      <c r="AX9" s="7"/>
       <c r="AY9" s="7"/>
       <c r="AZ9" s="7"/>
       <c r="BA9" s="7"/>
-      <c r="BB9" s="7"/>
-      <c r="BC9" s="4"/>
-      <c r="BE9" s="3">
+      <c r="BB9" s="4"/>
+      <c r="BD9" s="3">
         <v>4</v>
       </c>
-      <c r="BF9" s="7"/>
-      <c r="BG9" s="10"/>
-      <c r="BH9" s="7"/>
-      <c r="BI9" s="4"/>
-      <c r="BK9" s="3">
+      <c r="BE9" s="7"/>
+      <c r="BF9" s="10"/>
+      <c r="BG9" s="7"/>
+      <c r="BH9" s="4"/>
+      <c r="BJ9" s="3">
         <v>4</v>
       </c>
-      <c r="BL9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="BN9" s="3"/>
+      <c r="BK9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM9" s="3"/>
+      <c r="BN9" s="7"/>
       <c r="BO9" s="7"/>
       <c r="BP9" s="7"/>
       <c r="BQ9" s="7"/>
       <c r="BR9" s="7"/>
-      <c r="BS9" s="7"/>
-      <c r="BT9" s="4"/>
+      <c r="BS9" s="4"/>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>69</v>
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C10" s="3">
         <v>6</v>
@@ -1688,53 +1722,52 @@
       <c r="AD10" s="7"/>
       <c r="AE10" s="7"/>
       <c r="AF10" s="7"/>
-      <c r="AG10" s="7"/>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="4"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="4"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="4"/>
-      <c r="AQ10" s="3">
+      <c r="AG10" s="4"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="4"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="4"/>
+      <c r="AO10" s="3">
         <v>5</v>
       </c>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7"/>
       <c r="AR10" s="7"/>
       <c r="AS10" s="7"/>
       <c r="AT10" s="7"/>
-      <c r="AU10" s="7"/>
-      <c r="AV10" s="4"/>
-      <c r="AX10" s="3">
+      <c r="AU10" s="4"/>
+      <c r="AW10" s="3">
         <v>5</v>
       </c>
+      <c r="AX10" s="7"/>
       <c r="AY10" s="7"/>
       <c r="AZ10" s="7"/>
       <c r="BA10" s="7"/>
-      <c r="BB10" s="7"/>
-      <c r="BC10" s="4"/>
-      <c r="BE10" s="3">
+      <c r="BB10" s="4"/>
+      <c r="BD10" s="3">
         <v>5</v>
       </c>
-      <c r="BF10" s="7"/>
-      <c r="BG10" s="10"/>
-      <c r="BH10" s="7"/>
-      <c r="BI10" s="4"/>
-      <c r="BK10" s="3">
+      <c r="BE10" s="7"/>
+      <c r="BF10" s="10"/>
+      <c r="BG10" s="7"/>
+      <c r="BH10" s="4"/>
+      <c r="BJ10" s="3">
         <v>5</v>
       </c>
-      <c r="BL10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="BN10" s="3"/>
+      <c r="BK10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BM10" s="3"/>
+      <c r="BN10" s="7"/>
       <c r="BO10" s="7"/>
       <c r="BP10" s="7"/>
       <c r="BQ10" s="7"/>
       <c r="BR10" s="7"/>
-      <c r="BS10" s="7"/>
-      <c r="BT10" s="4"/>
+      <c r="BS10" s="4"/>
     </row>
-    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>86</v>
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="3">
         <v>7</v>
@@ -1767,49 +1800,48 @@
       <c r="AD11" s="7"/>
       <c r="AE11" s="7"/>
       <c r="AF11" s="7"/>
-      <c r="AG11" s="7"/>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="4"/>
-      <c r="AK11" s="3"/>
-      <c r="AL11" s="4"/>
-      <c r="AN11" s="3"/>
-      <c r="AO11" s="4"/>
-      <c r="AQ11" s="3">
+      <c r="AG11" s="4"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="4"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="4"/>
+      <c r="AO11" s="3">
         <v>6</v>
       </c>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7"/>
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
       <c r="AT11" s="7"/>
-      <c r="AU11" s="7"/>
-      <c r="AV11" s="4"/>
-      <c r="AX11" s="3">
+      <c r="AU11" s="4"/>
+      <c r="AW11" s="3">
         <v>6</v>
       </c>
+      <c r="AX11" s="7"/>
       <c r="AY11" s="7"/>
       <c r="AZ11" s="7"/>
       <c r="BA11" s="7"/>
-      <c r="BB11" s="7"/>
-      <c r="BC11" s="4"/>
-      <c r="BE11" s="3">
+      <c r="BB11" s="4"/>
+      <c r="BD11" s="3">
         <v>6</v>
       </c>
-      <c r="BF11" s="7"/>
-      <c r="BG11" s="10"/>
-      <c r="BH11" s="7"/>
-      <c r="BI11" s="4"/>
-      <c r="BK11" s="3"/>
-      <c r="BL11" s="4"/>
-      <c r="BN11" s="3"/>
+      <c r="BE11" s="7"/>
+      <c r="BF11" s="10"/>
+      <c r="BG11" s="7"/>
+      <c r="BH11" s="4"/>
+      <c r="BJ11" s="3"/>
+      <c r="BK11" s="4"/>
+      <c r="BM11" s="3"/>
+      <c r="BN11" s="7"/>
       <c r="BO11" s="7"/>
       <c r="BP11" s="7"/>
       <c r="BQ11" s="7"/>
       <c r="BR11" s="7"/>
-      <c r="BS11" s="7"/>
-      <c r="BT11" s="4"/>
+      <c r="BS11" s="4"/>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>23</v>
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>8</v>
@@ -1842,49 +1874,48 @@
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
-      <c r="AG12" s="7"/>
-      <c r="AH12" s="7"/>
-      <c r="AI12" s="4"/>
-      <c r="AK12" s="3"/>
-      <c r="AL12" s="4"/>
-      <c r="AN12" s="3"/>
-      <c r="AO12" s="4"/>
-      <c r="AQ12" s="3">
+      <c r="AG12" s="4"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="4"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="4"/>
+      <c r="AO12" s="3">
         <v>7</v>
       </c>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7"/>
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
       <c r="AT12" s="7"/>
-      <c r="AU12" s="7"/>
-      <c r="AV12" s="4"/>
-      <c r="AX12" s="3">
+      <c r="AU12" s="4"/>
+      <c r="AW12" s="3">
         <v>7</v>
       </c>
+      <c r="AX12" s="7"/>
       <c r="AY12" s="7"/>
       <c r="AZ12" s="7"/>
       <c r="BA12" s="7"/>
-      <c r="BB12" s="7"/>
-      <c r="BC12" s="4"/>
-      <c r="BE12" s="3">
+      <c r="BB12" s="4"/>
+      <c r="BD12" s="3">
         <v>7</v>
       </c>
-      <c r="BF12" s="7"/>
-      <c r="BG12" s="10"/>
-      <c r="BH12" s="7"/>
-      <c r="BI12" s="4"/>
-      <c r="BK12" s="3"/>
-      <c r="BL12" s="4"/>
-      <c r="BN12" s="3"/>
+      <c r="BE12" s="7"/>
+      <c r="BF12" s="10"/>
+      <c r="BG12" s="7"/>
+      <c r="BH12" s="4"/>
+      <c r="BJ12" s="3"/>
+      <c r="BK12" s="4"/>
+      <c r="BM12" s="3"/>
+      <c r="BN12" s="7"/>
       <c r="BO12" s="7"/>
       <c r="BP12" s="7"/>
       <c r="BQ12" s="7"/>
       <c r="BR12" s="7"/>
-      <c r="BS12" s="7"/>
-      <c r="BT12" s="4"/>
+      <c r="BS12" s="4"/>
     </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>14</v>
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="C13" s="3">
         <v>9</v>
@@ -1915,49 +1946,48 @@
       <c r="AD13" s="7"/>
       <c r="AE13" s="7"/>
       <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
-      <c r="AH13" s="7"/>
-      <c r="AI13" s="4"/>
-      <c r="AK13" s="3"/>
-      <c r="AL13" s="4"/>
-      <c r="AN13" s="3"/>
-      <c r="AO13" s="4"/>
-      <c r="AQ13" s="3">
+      <c r="AG13" s="4"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="4"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="4"/>
+      <c r="AO13" s="3">
         <v>8</v>
       </c>
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7"/>
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
       <c r="AT13" s="7"/>
-      <c r="AU13" s="7"/>
-      <c r="AV13" s="4"/>
-      <c r="AX13" s="3">
+      <c r="AU13" s="4"/>
+      <c r="AW13" s="3">
         <v>8</v>
       </c>
+      <c r="AX13" s="7"/>
       <c r="AY13" s="7"/>
       <c r="AZ13" s="7"/>
       <c r="BA13" s="7"/>
-      <c r="BB13" s="7"/>
-      <c r="BC13" s="4"/>
-      <c r="BE13" s="3">
+      <c r="BB13" s="4"/>
+      <c r="BD13" s="3">
         <v>8</v>
       </c>
-      <c r="BF13" s="7"/>
-      <c r="BG13" s="10"/>
-      <c r="BH13" s="7"/>
-      <c r="BI13" s="4"/>
-      <c r="BK13" s="3"/>
-      <c r="BL13" s="4"/>
-      <c r="BN13" s="3"/>
+      <c r="BE13" s="7"/>
+      <c r="BF13" s="10"/>
+      <c r="BG13" s="7"/>
+      <c r="BH13" s="4"/>
+      <c r="BJ13" s="3"/>
+      <c r="BK13" s="4"/>
+      <c r="BM13" s="3"/>
+      <c r="BN13" s="7"/>
       <c r="BO13" s="7"/>
       <c r="BP13" s="7"/>
       <c r="BQ13" s="7"/>
       <c r="BR13" s="7"/>
-      <c r="BS13" s="7"/>
-      <c r="BT13" s="4"/>
+      <c r="BS13" s="4"/>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>77</v>
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="C14" s="3">
         <v>10</v>
@@ -1988,49 +2018,48 @@
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
       <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="4"/>
-      <c r="AK14" s="3"/>
-      <c r="AL14" s="4"/>
-      <c r="AN14" s="3"/>
-      <c r="AO14" s="4"/>
-      <c r="AQ14" s="3">
+      <c r="AG14" s="4"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="4"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="4"/>
+      <c r="AO14" s="3">
         <v>9</v>
       </c>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
       <c r="AT14" s="7"/>
-      <c r="AU14" s="7"/>
-      <c r="AV14" s="4"/>
-      <c r="AX14" s="3">
+      <c r="AU14" s="4"/>
+      <c r="AW14" s="3">
         <v>9</v>
       </c>
+      <c r="AX14" s="7"/>
       <c r="AY14" s="7"/>
       <c r="AZ14" s="7"/>
       <c r="BA14" s="7"/>
-      <c r="BB14" s="7"/>
-      <c r="BC14" s="4"/>
-      <c r="BE14" s="3">
+      <c r="BB14" s="4"/>
+      <c r="BD14" s="3">
         <v>9</v>
       </c>
-      <c r="BF14" s="7"/>
-      <c r="BG14" s="10"/>
-      <c r="BH14" s="7"/>
-      <c r="BI14" s="4"/>
-      <c r="BK14" s="3"/>
-      <c r="BL14" s="4"/>
-      <c r="BN14" s="3"/>
+      <c r="BE14" s="7"/>
+      <c r="BF14" s="10"/>
+      <c r="BG14" s="7"/>
+      <c r="BH14" s="4"/>
+      <c r="BJ14" s="3"/>
+      <c r="BK14" s="4"/>
+      <c r="BM14" s="3"/>
+      <c r="BN14" s="7"/>
       <c r="BO14" s="7"/>
       <c r="BP14" s="7"/>
       <c r="BQ14" s="7"/>
       <c r="BR14" s="7"/>
-      <c r="BS14" s="7"/>
-      <c r="BT14" s="4"/>
+      <c r="BS14" s="4"/>
     </row>
-    <row r="15" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
-        <v>65</v>
+    <row r="15" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C15" s="5">
         <v>11</v>
@@ -2061,73 +2090,72 @@
       <c r="AD15" s="9"/>
       <c r="AE15" s="9"/>
       <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="6"/>
-      <c r="AK15" s="5"/>
-      <c r="AL15" s="6"/>
-      <c r="AN15" s="5"/>
-      <c r="AO15" s="6"/>
-      <c r="AQ15" s="5">
+      <c r="AG15" s="6"/>
+      <c r="AI15" s="5"/>
+      <c r="AJ15" s="6"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="6"/>
+      <c r="AO15" s="5">
         <v>10</v>
       </c>
+      <c r="AP15" s="9"/>
+      <c r="AQ15" s="9"/>
       <c r="AR15" s="9"/>
       <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
-      <c r="AU15" s="9"/>
-      <c r="AV15" s="6"/>
-      <c r="AX15" s="5">
+      <c r="AU15" s="6"/>
+      <c r="AW15" s="5">
         <v>10</v>
       </c>
+      <c r="AX15" s="9"/>
       <c r="AY15" s="9"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="9"/>
-      <c r="BB15" s="9"/>
-      <c r="BC15" s="6"/>
-      <c r="BE15" s="5">
+      <c r="BB15" s="6"/>
+      <c r="BD15" s="5">
         <v>10</v>
       </c>
-      <c r="BF15" s="9"/>
-      <c r="BG15" s="11"/>
-      <c r="BH15" s="9"/>
-      <c r="BI15" s="6"/>
-      <c r="BK15" s="5"/>
-      <c r="BL15" s="6"/>
-      <c r="BN15" s="5"/>
+      <c r="BE15" s="9"/>
+      <c r="BF15" s="11"/>
+      <c r="BG15" s="9"/>
+      <c r="BH15" s="6"/>
+      <c r="BJ15" s="5"/>
+      <c r="BK15" s="6"/>
+      <c r="BM15" s="5"/>
+      <c r="BN15" s="9"/>
       <c r="BO15" s="9"/>
       <c r="BP15" s="9"/>
       <c r="BQ15" s="9"/>
       <c r="BR15" s="9"/>
-      <c r="BS15" s="9"/>
-      <c r="BT15" s="6"/>
+      <c r="BS15" s="6"/>
     </row>
-    <row r="16" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>78</v>
+    <row r="16" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="AE16" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="BN3:BT3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="BM3:BS3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AI3:AJ3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="AX3:BC3"/>
-    <mergeCell ref="BE3:BI3"/>
-    <mergeCell ref="AQ3:AV3"/>
-    <mergeCell ref="BK3:BL3"/>
+    <mergeCell ref="AW3:BB3"/>
+    <mergeCell ref="BD3:BH3"/>
+    <mergeCell ref="AO3:AU3"/>
+    <mergeCell ref="BJ3:BK3"/>
     <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Y3:AI3"/>
+    <mergeCell ref="Y3:AG3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AS5" r:id="rId1"/>
-    <hyperlink ref="AS6" r:id="rId2"/>
+    <hyperlink ref="AR5" r:id="rId1"/>
+    <hyperlink ref="AR6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
altered excel table to match changed made to SQL database
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
   <si>
     <t>fries</t>
   </si>
@@ -212,9 +212,6 @@
     <t>delivery_timestamp</t>
   </si>
   <si>
-    <t>payment_id</t>
-  </si>
-  <si>
     <t>instructions</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
     <t>delivery_statuses</t>
   </si>
   <si>
-    <t>selivery_status_is</t>
-  </si>
-  <si>
     <t>delivery_status</t>
   </si>
   <si>
@@ -330,6 +324,9 @@
   </si>
   <si>
     <t>close_time</t>
+  </si>
+  <si>
+    <t>delivery_status_is</t>
   </si>
 </sst>
 </file>
@@ -848,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM1" workbookViewId="0">
-      <selection activeCell="BS13" sqref="BS13"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AZ21" sqref="AZ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +867,7 @@
     <col min="26" max="26" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -946,15 +943,15 @@
       <c r="AF3" s="19"/>
       <c r="AG3" s="20"/>
       <c r="AI3" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AJ3" s="23"/>
       <c r="AL3" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AM3" s="23"/>
       <c r="AO3" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AP3" s="19"/>
       <c r="AQ3" s="19"/>
@@ -963,7 +960,7 @@
       <c r="AT3" s="19"/>
       <c r="AU3" s="20"/>
       <c r="AW3" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="19"/>
       <c r="AY3" s="19"/>
@@ -971,18 +968,18 @@
       <c r="BA3" s="19"/>
       <c r="BB3" s="20"/>
       <c r="BD3" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="BE3" s="19"/>
       <c r="BF3" s="19"/>
       <c r="BG3" s="19"/>
       <c r="BH3" s="20"/>
       <c r="BJ3" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="BK3" s="20"/>
       <c r="BM3" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="BN3" s="22"/>
       <c r="BO3" s="22"/>
@@ -1059,112 +1056,112 @@
         <v>61</v>
       </c>
       <c r="AC4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AG4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AG4" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="AI4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="AO4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="AP4" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AQ4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AR4" s="8" t="s">
+      <c r="AT4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AS4" s="8" t="s">
+      <c r="AU4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AT4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU4" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="AW4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AX4" s="8" t="s">
+      <c r="AZ4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AY4" s="8" t="s">
+      <c r="BA4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AZ4" s="8" t="s">
+      <c r="BB4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="BA4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="BB4" s="2" t="s">
+      <c r="BD4" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="BD4" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="BE4" s="8" t="s">
         <v>59</v>
       </c>
       <c r="BF4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="BG4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="BH4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BG4" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="BH4" s="2" t="s">
+      <c r="BJ4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BJ4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BK4" s="2" t="s">
+      <c r="BM4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="BO4" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="BM4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BN4" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="BO4" s="8" t="s">
+      <c r="BP4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="BQ4" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="BP4" s="14" t="s">
+      <c r="BR4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="BQ4" s="14" t="s">
+      <c r="BS4" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="BR4" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="BS4" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:71" x14ac:dyDescent="0.25">
@@ -1239,10 +1236,10 @@
         <v>0</v>
       </c>
       <c r="AP5" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AQ5" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AR5" s="13" t="s">
         <v>12</v>
@@ -1355,10 +1352,10 @@
         <v>1</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AQ6" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AR6" s="13" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
added UserService and other misc changes
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syntel.MININT-1GOAKQE\Documents\Git\CaseStudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syntel.MININT-DO5C1AM\Documents\CaseStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
   <si>
     <t>fries</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>delivery_status_is</t>
+  </si>
+  <si>
+    <t>delivery_methods</t>
   </si>
 </sst>
 </file>
@@ -845,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AZ21" sqref="AZ21"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BF5" sqref="BF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +950,7 @@
       </c>
       <c r="AJ3" s="23"/>
       <c r="AL3" s="21" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="AM3" s="23"/>
       <c r="AO3" s="18" t="s">

</xml_diff>

<commit_message>
Altered table definitions in excel to meet new
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syntel.MININT-DO5C1AM\Documents\CaseStudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syntel.MININT-1GOAKQE\Documents\Git\CaseStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
   <si>
     <t>fries</t>
   </si>
@@ -330,6 +330,30 @@
   </si>
   <si>
     <t>delivery_methods</t>
+  </si>
+  <si>
+    <t>item_types</t>
+  </si>
+  <si>
+    <t>item_type_id</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>entrée</t>
+  </si>
+  <si>
+    <t>combo</t>
+  </si>
+  <si>
+    <t>User_id</t>
+  </si>
+  <si>
+    <t>phone</t>
   </si>
 </sst>
 </file>
@@ -361,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -523,12 +547,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -565,6 +620,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -846,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BS16"/>
+  <dimension ref="A2:BY16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BF5" sqref="BF5"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AW22" sqref="AW22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,53 +916,54 @@
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11" customWidth="1"/>
-    <col min="44" max="44" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="11" customWidth="1"/>
+    <col min="49" max="49" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>30</v>
       </c>
@@ -915,83 +975,89 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="K3" s="21" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="L3" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="O3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="N3" s="18" t="s">
+      <c r="P3" s="23"/>
+      <c r="R3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="Q3" s="18" t="s">
+      <c r="S3" s="20"/>
+      <c r="U3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="20"/>
-      <c r="V3" s="18" t="s">
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="20"/>
+      <c r="Z3" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="20"/>
-      <c r="Y3" s="18" t="s">
+      <c r="AA3" s="20"/>
+      <c r="AC3" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
       <c r="AD3" s="19"/>
       <c r="AE3" s="19"/>
       <c r="AF3" s="19"/>
-      <c r="AG3" s="20"/>
-      <c r="AI3" s="21" t="s">
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="19"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="20"/>
+      <c r="AM3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AJ3" s="23"/>
-      <c r="AL3" s="21" t="s">
+      <c r="AN3" s="23"/>
+      <c r="AP3" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="AM3" s="23"/>
-      <c r="AO3" s="18" t="s">
+      <c r="AQ3" s="23"/>
+      <c r="AS3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AP3" s="19"/>
-      <c r="AQ3" s="19"/>
-      <c r="AR3" s="19"/>
-      <c r="AS3" s="19"/>
       <c r="AT3" s="19"/>
-      <c r="AU3" s="20"/>
-      <c r="AW3" s="18" t="s">
-        <v>80</v>
-      </c>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AW3" s="19"/>
       <c r="AX3" s="19"/>
       <c r="AY3" s="19"/>
-      <c r="AZ3" s="19"/>
-      <c r="BA3" s="19"/>
-      <c r="BB3" s="20"/>
-      <c r="BD3" s="18" t="s">
-        <v>87</v>
-      </c>
+      <c r="BB3" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
       <c r="BE3" s="19"/>
       <c r="BF3" s="19"/>
       <c r="BG3" s="19"/>
       <c r="BH3" s="20"/>
       <c r="BJ3" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK3" s="19"/>
+      <c r="BL3" s="19"/>
+      <c r="BM3" s="19"/>
+      <c r="BN3" s="20"/>
+      <c r="BP3" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="BK3" s="20"/>
-      <c r="BM3" s="21" t="s">
+      <c r="BQ3" s="20"/>
+      <c r="BS3" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="BN3" s="22"/>
-      <c r="BO3" s="22"/>
-      <c r="BP3" s="22"/>
-      <c r="BQ3" s="22"/>
-      <c r="BR3" s="22"/>
-      <c r="BS3" s="23"/>
+      <c r="BT3" s="22"/>
+      <c r="BU3" s="22"/>
+      <c r="BV3" s="22"/>
+      <c r="BW3" s="22"/>
+      <c r="BX3" s="22"/>
+      <c r="BY3" s="23"/>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1005,169 +1071,181 @@
         <v>43</v>
       </c>
       <c r="F4" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AH4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AI4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AJ4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AG4" s="2" t="s">
+      <c r="AK4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AJ4" s="2" t="s">
+      <c r="AN4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AM4" s="2" t="s">
+      <c r="AQ4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AT4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AQ4" s="8" t="s">
+      <c r="AU4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AR4" s="8" t="s">
+      <c r="AV4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AW4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="AS4" s="8" t="s">
+      <c r="AX4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AT4" s="8" t="s">
+      <c r="AY4" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AU4" s="2" t="s">
+      <c r="BB4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AW4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX4" s="8" t="s">
+      <c r="BC4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="BD4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AY4" s="8" t="s">
+      <c r="BE4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AZ4" s="8" t="s">
+      <c r="BF4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BA4" s="8" t="s">
+      <c r="BG4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="BB4" s="2" t="s">
+      <c r="BH4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="BD4" s="1" t="s">
+      <c r="BJ4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BE4" s="8" t="s">
+      <c r="BK4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="BF4" s="8" t="s">
+      <c r="BL4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="BG4" s="8" t="s">
+      <c r="BM4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="BH4" s="2" t="s">
+      <c r="BN4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BJ4" s="1" t="s">
+      <c r="BP4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BK4" s="2" t="s">
+      <c r="BQ4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BM4" s="1" t="s">
+      <c r="BS4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN4" s="8" t="s">
+      <c r="BT4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="BO4" s="8" t="s">
+      <c r="BU4" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="BP4" s="14" t="s">
+      <c r="BV4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="BQ4" s="14" t="s">
+      <c r="BW4" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="BR4" s="8" t="s">
+      <c r="BX4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="BS4" s="2" t="s">
+      <c r="BY4" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>39</v>
       </c>
@@ -1183,115 +1261,125 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="4"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4"/>
-      <c r="N5" s="3">
+      <c r="I5" s="7"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="R5" s="3">
         <v>4</v>
       </c>
-      <c r="O5" s="4">
+      <c r="S5" s="4">
         <v>1</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="U5" s="3">
         <v>0</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="V5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="W5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="3">
+      <c r="Z5" s="3">
         <v>2</v>
       </c>
-      <c r="W5" s="4">
+      <c r="AA5" s="4">
         <v>3</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="AC5" s="3">
         <v>0</v>
       </c>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
-      <c r="AE5" s="7">
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7">
         <v>1</v>
       </c>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="4"/>
-      <c r="AI5" s="3">
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="4"/>
+      <c r="AM5" s="3">
         <v>0</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AL5" s="3">
+      <c r="AP5" s="3">
         <v>0</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AO5" s="3">
+      <c r="AS5" s="3">
         <v>0</v>
       </c>
-      <c r="AP5" s="7" t="s">
+      <c r="AT5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AQ5" s="7" t="s">
+      <c r="AU5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="AR5" s="13" t="s">
+      <c r="AV5" s="7"/>
+      <c r="AW5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="AS5" s="7"/>
-      <c r="AT5" s="7">
+      <c r="AX5" s="7"/>
+      <c r="AY5" s="25">
         <v>1</v>
       </c>
-      <c r="AU5" s="4"/>
-      <c r="AW5" s="3">
+      <c r="BB5" s="3">
         <v>0</v>
       </c>
-      <c r="AX5" s="7"/>
-      <c r="AY5" s="7"/>
-      <c r="AZ5" s="7" t="s">
+      <c r="BC5" s="7">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="7"/>
+      <c r="BE5" s="7"/>
+      <c r="BF5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="BA5" s="7"/>
-      <c r="BB5" s="4"/>
-      <c r="BD5" s="3">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="7">
-        <v>1</v>
-      </c>
-      <c r="BF5" s="10">
-        <v>554466778899</v>
-      </c>
-      <c r="BG5" s="12">
-        <v>43718</v>
-      </c>
-      <c r="BH5" s="4">
-        <v>234</v>
-      </c>
+      <c r="BG5" s="7"/>
+      <c r="BH5" s="4"/>
       <c r="BJ5" s="3">
         <v>0</v>
       </c>
-      <c r="BK5" s="4" t="s">
+      <c r="BK5" s="7">
+        <v>1</v>
+      </c>
+      <c r="BL5" s="10">
+        <v>554466778899</v>
+      </c>
+      <c r="BM5" s="12">
+        <v>43718</v>
+      </c>
+      <c r="BN5" s="4">
+        <v>234</v>
+      </c>
+      <c r="BP5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="BM5" s="3"/>
-      <c r="BN5" s="7"/>
-      <c r="BO5" s="7"/>
-      <c r="BP5" s="7"/>
-      <c r="BQ5" s="7"/>
-      <c r="BR5" s="7"/>
-      <c r="BS5" s="4"/>
+      <c r="BS5" s="3"/>
+      <c r="BT5" s="7"/>
+      <c r="BU5" s="7"/>
+      <c r="BV5" s="7"/>
+      <c r="BW5" s="7"/>
+      <c r="BX5" s="7"/>
+      <c r="BY5" s="4"/>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
@@ -1307,105 +1395,115 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="4"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="4"/>
-      <c r="N6" s="3">
+      <c r="I6" s="7"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="3">
+        <v>2</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="4"/>
+      <c r="R6" s="3">
         <v>4</v>
       </c>
-      <c r="O6" s="4">
+      <c r="S6" s="4">
         <v>2</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="U6" s="3">
         <v>1</v>
       </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="4"/>
-      <c r="V6" s="3">
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="4"/>
+      <c r="Z6" s="3">
         <v>2</v>
       </c>
-      <c r="W6" s="4">
+      <c r="AA6" s="4">
         <v>4</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="AC6" s="3">
         <v>1</v>
       </c>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
-      <c r="AG6" s="4"/>
-      <c r="AI6" s="3">
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="4"/>
+      <c r="AM6" s="3">
         <v>1</v>
       </c>
-      <c r="AJ6" s="4" t="s">
+      <c r="AN6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL6" s="3">
+      <c r="AP6" s="3">
         <v>1</v>
       </c>
-      <c r="AM6" s="4" t="s">
+      <c r="AQ6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AO6" s="3">
+      <c r="AS6" s="3">
         <v>1</v>
       </c>
-      <c r="AP6" s="7" t="s">
+      <c r="AT6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AQ6" s="7" t="s">
+      <c r="AU6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AR6" s="13" t="s">
+      <c r="AV6" s="7"/>
+      <c r="AW6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AS6" s="7"/>
-      <c r="AT6" s="7">
+      <c r="AX6" s="7"/>
+      <c r="AY6" s="25">
         <v>0</v>
       </c>
-      <c r="AU6" s="4"/>
-      <c r="AW6" s="3">
+      <c r="BB6" s="3">
         <v>1</v>
       </c>
-      <c r="AX6" s="7"/>
-      <c r="AY6" s="7"/>
-      <c r="AZ6" s="7"/>
-      <c r="BA6" s="7"/>
-      <c r="BB6" s="4"/>
-      <c r="BD6" s="3">
-        <v>1</v>
-      </c>
-      <c r="BE6" s="7">
-        <v>1</v>
-      </c>
-      <c r="BF6" s="10">
-        <v>683967034588</v>
-      </c>
-      <c r="BG6" s="12">
-        <v>43957</v>
-      </c>
-      <c r="BH6" s="4">
-        <v>354</v>
-      </c>
+      <c r="BC6" s="7">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="7"/>
+      <c r="BE6" s="7"/>
+      <c r="BF6" s="7"/>
+      <c r="BG6" s="7"/>
+      <c r="BH6" s="4"/>
       <c r="BJ6" s="3">
         <v>1</v>
       </c>
-      <c r="BK6" s="4" t="s">
+      <c r="BK6" s="7">
+        <v>1</v>
+      </c>
+      <c r="BL6" s="10">
+        <v>683967034588</v>
+      </c>
+      <c r="BM6" s="12">
+        <v>43957</v>
+      </c>
+      <c r="BN6" s="4">
+        <v>354</v>
+      </c>
+      <c r="BP6" s="3">
+        <v>1</v>
+      </c>
+      <c r="BQ6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BM6" s="3"/>
-      <c r="BN6" s="7"/>
-      <c r="BO6" s="7"/>
-      <c r="BP6" s="7"/>
-      <c r="BQ6" s="7"/>
-      <c r="BR6" s="7"/>
-      <c r="BS6" s="4"/>
+      <c r="BS6" s="3"/>
+      <c r="BT6" s="7"/>
+      <c r="BU6" s="7"/>
+      <c r="BV6" s="7"/>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7"/>
+      <c r="BY6" s="4"/>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
@@ -1421,97 +1519,107 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="4"/>
-      <c r="N7" s="3">
+      <c r="I7" s="7"/>
+      <c r="J7" s="4"/>
+      <c r="L7" s="3">
+        <v>3</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="4"/>
+      <c r="R7" s="3">
         <v>4</v>
       </c>
-      <c r="O7" s="4">
+      <c r="S7" s="4">
         <v>3</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="U7" s="3">
         <v>2</v>
       </c>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="4"/>
-      <c r="V7" s="3">
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="4"/>
+      <c r="Z7" s="3">
         <v>2</v>
       </c>
-      <c r="W7" s="4">
+      <c r="AA7" s="4">
         <v>5</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="AC7" s="3">
         <v>2</v>
       </c>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
-      <c r="AG7" s="4"/>
-      <c r="AI7" s="3">
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="4"/>
+      <c r="AM7" s="3">
         <v>2</v>
       </c>
-      <c r="AJ7" s="4" t="s">
+      <c r="AN7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL7" s="3">
+      <c r="AP7" s="3">
         <v>2</v>
       </c>
-      <c r="AM7" s="4" t="s">
+      <c r="AQ7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AO7" s="3">
+      <c r="AS7" s="3">
         <v>2</v>
       </c>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-      <c r="AR7" s="7"/>
-      <c r="AS7" s="7"/>
       <c r="AT7" s="7"/>
-      <c r="AU7" s="4"/>
-      <c r="AW7" s="3">
+      <c r="AU7" s="7"/>
+      <c r="AV7" s="7"/>
+      <c r="AW7" s="7"/>
+      <c r="AX7" s="7"/>
+      <c r="AY7" s="25"/>
+      <c r="BB7" s="3">
         <v>2</v>
       </c>
-      <c r="AX7" s="7"/>
-      <c r="AY7" s="7"/>
-      <c r="AZ7" s="7"/>
-      <c r="BA7" s="7"/>
-      <c r="BB7" s="4"/>
-      <c r="BD7" s="3">
-        <v>2</v>
-      </c>
-      <c r="BE7" s="7">
-        <v>2</v>
-      </c>
-      <c r="BF7" s="10">
-        <v>338744976569</v>
-      </c>
-      <c r="BG7" s="12">
-        <v>45770</v>
-      </c>
-      <c r="BH7" s="4">
-        <v>325</v>
-      </c>
+      <c r="BC7" s="7">
+        <v>1</v>
+      </c>
+      <c r="BD7" s="7"/>
+      <c r="BE7" s="7"/>
+      <c r="BF7" s="7"/>
+      <c r="BG7" s="7"/>
+      <c r="BH7" s="4"/>
       <c r="BJ7" s="3">
         <v>2</v>
       </c>
-      <c r="BK7" s="4" t="s">
+      <c r="BK7" s="7">
+        <v>2</v>
+      </c>
+      <c r="BL7" s="10">
+        <v>338744976569</v>
+      </c>
+      <c r="BM7" s="12">
+        <v>45770</v>
+      </c>
+      <c r="BN7" s="4">
+        <v>325</v>
+      </c>
+      <c r="BP7" s="3">
+        <v>2</v>
+      </c>
+      <c r="BQ7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="BM7" s="3"/>
-      <c r="BN7" s="7"/>
-      <c r="BO7" s="7"/>
-      <c r="BP7" s="7"/>
-      <c r="BQ7" s="7"/>
-      <c r="BR7" s="7"/>
-      <c r="BS7" s="4"/>
+      <c r="BS7" s="3"/>
+      <c r="BT7" s="7"/>
+      <c r="BU7" s="7"/>
+      <c r="BV7" s="7"/>
+      <c r="BW7" s="7"/>
+      <c r="BX7" s="7"/>
+      <c r="BY7" s="4"/>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
@@ -1525,85 +1633,91 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="4"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4"/>
-      <c r="N8" s="3">
+      <c r="I8" s="7"/>
+      <c r="J8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="4"/>
+      <c r="R8" s="3">
         <v>5</v>
       </c>
-      <c r="O8" s="4">
+      <c r="S8" s="4">
         <v>1</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="U8" s="3">
         <v>3</v>
       </c>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="4"/>
-      <c r="V8" s="3">
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="4"/>
+      <c r="Z8" s="3">
         <v>2</v>
       </c>
-      <c r="W8" s="4">
+      <c r="AA8" s="4">
         <v>1</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="AC8" s="3">
         <v>3</v>
       </c>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="7"/>
-      <c r="AG8" s="4"/>
-      <c r="AI8" s="3">
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="4"/>
+      <c r="AM8" s="3">
         <v>3</v>
       </c>
-      <c r="AJ8" s="4" t="s">
+      <c r="AN8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="4"/>
-      <c r="AO8" s="3">
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="4"/>
+      <c r="AS8" s="3">
         <v>3</v>
       </c>
-      <c r="AP8" s="7"/>
-      <c r="AQ8" s="7"/>
-      <c r="AR8" s="7"/>
-      <c r="AS8" s="7"/>
       <c r="AT8" s="7"/>
-      <c r="AU8" s="4"/>
-      <c r="AW8" s="3">
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="7"/>
+      <c r="AX8" s="7"/>
+      <c r="AY8" s="25"/>
+      <c r="BB8" s="3">
         <v>3</v>
       </c>
-      <c r="AX8" s="7"/>
-      <c r="AY8" s="7"/>
-      <c r="AZ8" s="7"/>
-      <c r="BA8" s="7"/>
-      <c r="BB8" s="4"/>
-      <c r="BD8" s="3">
-        <v>3</v>
-      </c>
+      <c r="BC8" s="27">
+        <v>1</v>
+      </c>
+      <c r="BD8" s="7"/>
       <c r="BE8" s="7"/>
-      <c r="BF8" s="10"/>
+      <c r="BF8" s="7"/>
       <c r="BG8" s="7"/>
       <c r="BH8" s="4"/>
       <c r="BJ8" s="3">
         <v>3</v>
       </c>
-      <c r="BK8" s="4" t="s">
+      <c r="BK8" s="7"/>
+      <c r="BL8" s="10"/>
+      <c r="BM8" s="7"/>
+      <c r="BN8" s="4"/>
+      <c r="BP8" s="3">
+        <v>3</v>
+      </c>
+      <c r="BQ8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="BM8" s="3"/>
-      <c r="BN8" s="7"/>
-      <c r="BO8" s="7"/>
-      <c r="BP8" s="7"/>
-      <c r="BQ8" s="7"/>
-      <c r="BR8" s="7"/>
-      <c r="BS8" s="4"/>
+      <c r="BS8" s="3"/>
+      <c r="BT8" s="7"/>
+      <c r="BU8" s="7"/>
+      <c r="BV8" s="7"/>
+      <c r="BW8" s="7"/>
+      <c r="BX8" s="7"/>
+      <c r="BY8" s="4"/>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
@@ -1617,77 +1731,81 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="4"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="4"/>
-      <c r="N9" s="3">
+      <c r="I9" s="7"/>
+      <c r="J9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="4"/>
+      <c r="R9" s="3">
         <v>5</v>
       </c>
-      <c r="O9" s="4">
+      <c r="S9" s="4">
         <v>4</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="U9" s="3">
         <v>4</v>
       </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="4"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="4"/>
-      <c r="Y9" s="3">
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="4"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="4"/>
+      <c r="AC9" s="3">
         <v>4</v>
       </c>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
-      <c r="AG9" s="4"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="4"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="4"/>
-      <c r="AO9" s="3">
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="4"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="4"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="4"/>
+      <c r="AS9" s="3">
         <v>4</v>
       </c>
-      <c r="AP9" s="7"/>
-      <c r="AQ9" s="7"/>
-      <c r="AR9" s="7"/>
-      <c r="AS9" s="7"/>
       <c r="AT9" s="7"/>
-      <c r="AU9" s="4"/>
-      <c r="AW9" s="3">
+      <c r="AU9" s="7"/>
+      <c r="AV9" s="7"/>
+      <c r="AW9" s="7"/>
+      <c r="AX9" s="7"/>
+      <c r="AY9" s="25"/>
+      <c r="BB9" s="3">
         <v>4</v>
       </c>
-      <c r="AX9" s="7"/>
-      <c r="AY9" s="7"/>
-      <c r="AZ9" s="7"/>
-      <c r="BA9" s="7"/>
-      <c r="BB9" s="4"/>
-      <c r="BD9" s="3">
-        <v>4</v>
-      </c>
+      <c r="BC9" s="7"/>
+      <c r="BD9" s="7"/>
       <c r="BE9" s="7"/>
-      <c r="BF9" s="10"/>
+      <c r="BF9" s="7"/>
       <c r="BG9" s="7"/>
       <c r="BH9" s="4"/>
       <c r="BJ9" s="3">
         <v>4</v>
       </c>
-      <c r="BK9" s="4" t="s">
+      <c r="BK9" s="7"/>
+      <c r="BL9" s="10"/>
+      <c r="BM9" s="7"/>
+      <c r="BN9" s="4"/>
+      <c r="BP9" s="3">
+        <v>4</v>
+      </c>
+      <c r="BQ9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="BM9" s="3"/>
-      <c r="BN9" s="7"/>
-      <c r="BO9" s="7"/>
-      <c r="BP9" s="7"/>
-      <c r="BQ9" s="7"/>
-      <c r="BR9" s="7"/>
-      <c r="BS9" s="4"/>
+      <c r="BS9" s="3"/>
+      <c r="BT9" s="7"/>
+      <c r="BU9" s="7"/>
+      <c r="BV9" s="7"/>
+      <c r="BW9" s="7"/>
+      <c r="BX9" s="7"/>
+      <c r="BY9" s="4"/>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>26</v>
       </c>
@@ -1699,73 +1817,77 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="4"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="4"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="4"/>
-      <c r="Q10" s="3">
+      <c r="I10" s="7"/>
+      <c r="J10" s="4"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="4"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="4"/>
+      <c r="U10" s="3">
         <v>5</v>
       </c>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="4"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="4"/>
-      <c r="Y10" s="3">
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="4"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="4"/>
+      <c r="AC10" s="3">
         <v>5</v>
       </c>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
       <c r="AE10" s="7"/>
       <c r="AF10" s="7"/>
-      <c r="AG10" s="4"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="4"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="4"/>
-      <c r="AO10" s="3">
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="4"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="4"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="4"/>
+      <c r="AS10" s="3">
         <v>5</v>
       </c>
-      <c r="AP10" s="7"/>
-      <c r="AQ10" s="7"/>
-      <c r="AR10" s="7"/>
-      <c r="AS10" s="7"/>
       <c r="AT10" s="7"/>
-      <c r="AU10" s="4"/>
-      <c r="AW10" s="3">
+      <c r="AU10" s="7"/>
+      <c r="AV10" s="7"/>
+      <c r="AW10" s="7"/>
+      <c r="AX10" s="7"/>
+      <c r="AY10" s="25"/>
+      <c r="BB10" s="3">
         <v>5</v>
       </c>
-      <c r="AX10" s="7"/>
-      <c r="AY10" s="7"/>
-      <c r="AZ10" s="7"/>
-      <c r="BA10" s="7"/>
-      <c r="BB10" s="4"/>
-      <c r="BD10" s="3">
-        <v>5</v>
-      </c>
+      <c r="BC10" s="7"/>
+      <c r="BD10" s="7"/>
       <c r="BE10" s="7"/>
-      <c r="BF10" s="10"/>
+      <c r="BF10" s="7"/>
       <c r="BG10" s="7"/>
       <c r="BH10" s="4"/>
       <c r="BJ10" s="3">
         <v>5</v>
       </c>
-      <c r="BK10" s="4" t="s">
+      <c r="BK10" s="7"/>
+      <c r="BL10" s="10"/>
+      <c r="BM10" s="7"/>
+      <c r="BN10" s="4"/>
+      <c r="BP10" s="3">
+        <v>5</v>
+      </c>
+      <c r="BQ10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="BM10" s="3"/>
-      <c r="BN10" s="7"/>
-      <c r="BO10" s="7"/>
-      <c r="BP10" s="7"/>
-      <c r="BQ10" s="7"/>
-      <c r="BR10" s="7"/>
-      <c r="BS10" s="4"/>
+      <c r="BS10" s="3"/>
+      <c r="BT10" s="7"/>
+      <c r="BU10" s="7"/>
+      <c r="BV10" s="7"/>
+      <c r="BW10" s="7"/>
+      <c r="BX10" s="7"/>
+      <c r="BY10" s="4"/>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>38</v>
       </c>
@@ -1777,69 +1899,73 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="4"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="4"/>
-      <c r="Q11" s="3">
+      <c r="I11" s="7"/>
+      <c r="J11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="4"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="4"/>
+      <c r="U11" s="3">
         <v>6</v>
       </c>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="4"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="4"/>
-      <c r="Y11" s="3">
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="4"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="4"/>
+      <c r="AC11" s="3">
         <v>6</v>
       </c>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
       <c r="AE11" s="7"/>
       <c r="AF11" s="7"/>
-      <c r="AG11" s="4"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="4"/>
-      <c r="AL11" s="3"/>
-      <c r="AM11" s="4"/>
-      <c r="AO11" s="3">
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="4"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="4"/>
+      <c r="AP11" s="3"/>
+      <c r="AQ11" s="4"/>
+      <c r="AS11" s="3">
         <v>6</v>
       </c>
-      <c r="AP11" s="7"/>
-      <c r="AQ11" s="7"/>
-      <c r="AR11" s="7"/>
-      <c r="AS11" s="7"/>
       <c r="AT11" s="7"/>
-      <c r="AU11" s="4"/>
-      <c r="AW11" s="3">
+      <c r="AU11" s="7"/>
+      <c r="AV11" s="7"/>
+      <c r="AW11" s="7"/>
+      <c r="AX11" s="7"/>
+      <c r="AY11" s="25"/>
+      <c r="BB11" s="3">
         <v>6</v>
       </c>
-      <c r="AX11" s="7"/>
-      <c r="AY11" s="7"/>
-      <c r="AZ11" s="7"/>
-      <c r="BA11" s="7"/>
-      <c r="BB11" s="4"/>
-      <c r="BD11" s="3">
-        <v>6</v>
-      </c>
+      <c r="BC11" s="7"/>
+      <c r="BD11" s="7"/>
       <c r="BE11" s="7"/>
-      <c r="BF11" s="10"/>
+      <c r="BF11" s="7"/>
       <c r="BG11" s="7"/>
       <c r="BH11" s="4"/>
-      <c r="BJ11" s="3"/>
-      <c r="BK11" s="4"/>
-      <c r="BM11" s="3"/>
-      <c r="BN11" s="7"/>
-      <c r="BO11" s="7"/>
-      <c r="BP11" s="7"/>
-      <c r="BQ11" s="7"/>
-      <c r="BR11" s="7"/>
-      <c r="BS11" s="4"/>
+      <c r="BJ11" s="3">
+        <v>6</v>
+      </c>
+      <c r="BK11" s="7"/>
+      <c r="BL11" s="10"/>
+      <c r="BM11" s="7"/>
+      <c r="BN11" s="4"/>
+      <c r="BP11" s="3"/>
+      <c r="BQ11" s="4"/>
+      <c r="BS11" s="3"/>
+      <c r="BT11" s="7"/>
+      <c r="BU11" s="7"/>
+      <c r="BV11" s="7"/>
+      <c r="BW11" s="7"/>
+      <c r="BX11" s="7"/>
+      <c r="BY11" s="4"/>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
@@ -1851,69 +1977,73 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="4"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="4"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="4"/>
-      <c r="Q12" s="3">
+      <c r="I12" s="7"/>
+      <c r="J12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="4"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="4"/>
+      <c r="U12" s="3">
         <v>7</v>
       </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="4"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="4"/>
-      <c r="Y12" s="3">
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="4"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="4"/>
+      <c r="AC12" s="3">
         <v>7</v>
       </c>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
-      <c r="AG12" s="4"/>
-      <c r="AI12" s="3"/>
-      <c r="AJ12" s="4"/>
-      <c r="AL12" s="3"/>
-      <c r="AM12" s="4"/>
-      <c r="AO12" s="3">
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="4"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="4"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="4"/>
+      <c r="AS12" s="3">
         <v>7</v>
       </c>
-      <c r="AP12" s="7"/>
-      <c r="AQ12" s="7"/>
-      <c r="AR12" s="7"/>
-      <c r="AS12" s="7"/>
       <c r="AT12" s="7"/>
-      <c r="AU12" s="4"/>
-      <c r="AW12" s="3">
+      <c r="AU12" s="7"/>
+      <c r="AV12" s="7"/>
+      <c r="AW12" s="7"/>
+      <c r="AX12" s="7"/>
+      <c r="AY12" s="25"/>
+      <c r="BB12" s="3">
         <v>7</v>
       </c>
-      <c r="AX12" s="7"/>
-      <c r="AY12" s="7"/>
-      <c r="AZ12" s="7"/>
-      <c r="BA12" s="7"/>
-      <c r="BB12" s="4"/>
-      <c r="BD12" s="3">
-        <v>7</v>
-      </c>
+      <c r="BC12" s="7"/>
+      <c r="BD12" s="7"/>
       <c r="BE12" s="7"/>
-      <c r="BF12" s="10"/>
+      <c r="BF12" s="7"/>
       <c r="BG12" s="7"/>
       <c r="BH12" s="4"/>
-      <c r="BJ12" s="3"/>
-      <c r="BK12" s="4"/>
-      <c r="BM12" s="3"/>
-      <c r="BN12" s="7"/>
-      <c r="BO12" s="7"/>
-      <c r="BP12" s="7"/>
-      <c r="BQ12" s="7"/>
-      <c r="BR12" s="7"/>
-      <c r="BS12" s="4"/>
+      <c r="BJ12" s="3">
+        <v>7</v>
+      </c>
+      <c r="BK12" s="7"/>
+      <c r="BL12" s="10"/>
+      <c r="BM12" s="7"/>
+      <c r="BN12" s="4"/>
+      <c r="BP12" s="3"/>
+      <c r="BQ12" s="4"/>
+      <c r="BS12" s="3"/>
+      <c r="BT12" s="7"/>
+      <c r="BU12" s="7"/>
+      <c r="BV12" s="7"/>
+      <c r="BW12" s="7"/>
+      <c r="BX12" s="7"/>
+      <c r="BY12" s="4"/>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>8</v>
       </c>
@@ -1925,67 +2055,71 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="4"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="4"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="4"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="4"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="4"/>
-      <c r="Y13" s="3">
+      <c r="I13" s="7"/>
+      <c r="J13" s="4"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="4"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="4"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="4"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="4"/>
+      <c r="AC13" s="3">
         <v>8</v>
       </c>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
       <c r="AE13" s="7"/>
       <c r="AF13" s="7"/>
-      <c r="AG13" s="4"/>
-      <c r="AI13" s="3"/>
-      <c r="AJ13" s="4"/>
-      <c r="AL13" s="3"/>
-      <c r="AM13" s="4"/>
-      <c r="AO13" s="3">
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="4"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="4"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="4"/>
+      <c r="AS13" s="3">
         <v>8</v>
       </c>
-      <c r="AP13" s="7"/>
-      <c r="AQ13" s="7"/>
-      <c r="AR13" s="7"/>
-      <c r="AS13" s="7"/>
       <c r="AT13" s="7"/>
-      <c r="AU13" s="4"/>
-      <c r="AW13" s="3">
+      <c r="AU13" s="7"/>
+      <c r="AV13" s="7"/>
+      <c r="AW13" s="7"/>
+      <c r="AX13" s="7"/>
+      <c r="AY13" s="25"/>
+      <c r="BB13" s="3">
         <v>8</v>
       </c>
-      <c r="AX13" s="7"/>
-      <c r="AY13" s="7"/>
-      <c r="AZ13" s="7"/>
-      <c r="BA13" s="7"/>
-      <c r="BB13" s="4"/>
-      <c r="BD13" s="3">
-        <v>8</v>
-      </c>
+      <c r="BC13" s="7"/>
+      <c r="BD13" s="7"/>
       <c r="BE13" s="7"/>
-      <c r="BF13" s="10"/>
+      <c r="BF13" s="7"/>
       <c r="BG13" s="7"/>
       <c r="BH13" s="4"/>
-      <c r="BJ13" s="3"/>
-      <c r="BK13" s="4"/>
-      <c r="BM13" s="3"/>
-      <c r="BN13" s="7"/>
-      <c r="BO13" s="7"/>
-      <c r="BP13" s="7"/>
-      <c r="BQ13" s="7"/>
-      <c r="BR13" s="7"/>
-      <c r="BS13" s="4"/>
+      <c r="BJ13" s="3">
+        <v>8</v>
+      </c>
+      <c r="BK13" s="7"/>
+      <c r="BL13" s="10"/>
+      <c r="BM13" s="7"/>
+      <c r="BN13" s="4"/>
+      <c r="BP13" s="3"/>
+      <c r="BQ13" s="4"/>
+      <c r="BS13" s="3"/>
+      <c r="BT13" s="7"/>
+      <c r="BU13" s="7"/>
+      <c r="BV13" s="7"/>
+      <c r="BW13" s="7"/>
+      <c r="BX13" s="7"/>
+      <c r="BY13" s="4"/>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>32</v>
       </c>
@@ -1997,67 +2131,71 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="4"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="4"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="4"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="4"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="4"/>
-      <c r="Y14" s="3">
+      <c r="I14" s="7"/>
+      <c r="J14" s="4"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="4"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="4"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="4"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="4"/>
+      <c r="AC14" s="3">
         <v>9</v>
       </c>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
       <c r="AF14" s="7"/>
-      <c r="AG14" s="4"/>
-      <c r="AI14" s="3"/>
-      <c r="AJ14" s="4"/>
-      <c r="AL14" s="3"/>
-      <c r="AM14" s="4"/>
-      <c r="AO14" s="3">
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="4"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="4"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="4"/>
+      <c r="AS14" s="3">
         <v>9</v>
       </c>
-      <c r="AP14" s="7"/>
-      <c r="AQ14" s="7"/>
-      <c r="AR14" s="7"/>
-      <c r="AS14" s="7"/>
       <c r="AT14" s="7"/>
-      <c r="AU14" s="4"/>
-      <c r="AW14" s="3">
+      <c r="AU14" s="7"/>
+      <c r="AV14" s="7"/>
+      <c r="AW14" s="7"/>
+      <c r="AX14" s="7"/>
+      <c r="AY14" s="25"/>
+      <c r="BB14" s="3">
         <v>9</v>
       </c>
-      <c r="AX14" s="7"/>
-      <c r="AY14" s="7"/>
-      <c r="AZ14" s="7"/>
-      <c r="BA14" s="7"/>
-      <c r="BB14" s="4"/>
-      <c r="BD14" s="3">
-        <v>9</v>
-      </c>
+      <c r="BC14" s="7"/>
+      <c r="BD14" s="7"/>
       <c r="BE14" s="7"/>
-      <c r="BF14" s="10"/>
+      <c r="BF14" s="7"/>
       <c r="BG14" s="7"/>
       <c r="BH14" s="4"/>
-      <c r="BJ14" s="3"/>
-      <c r="BK14" s="4"/>
-      <c r="BM14" s="3"/>
-      <c r="BN14" s="7"/>
-      <c r="BO14" s="7"/>
-      <c r="BP14" s="7"/>
-      <c r="BQ14" s="7"/>
-      <c r="BR14" s="7"/>
-      <c r="BS14" s="4"/>
+      <c r="BJ14" s="3">
+        <v>9</v>
+      </c>
+      <c r="BK14" s="7"/>
+      <c r="BL14" s="10"/>
+      <c r="BM14" s="7"/>
+      <c r="BN14" s="4"/>
+      <c r="BP14" s="3"/>
+      <c r="BQ14" s="4"/>
+      <c r="BS14" s="3"/>
+      <c r="BT14" s="7"/>
+      <c r="BU14" s="7"/>
+      <c r="BV14" s="7"/>
+      <c r="BW14" s="7"/>
+      <c r="BX14" s="7"/>
+      <c r="BY14" s="4"/>
     </row>
-    <row r="15" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>25</v>
       </c>
@@ -2069,93 +2207,98 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="6"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="6"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="6"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="6"/>
-      <c r="Y15" s="5">
+      <c r="I15" s="9"/>
+      <c r="J15" s="6"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="6"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="6"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="6"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="6"/>
+      <c r="AC15" s="5">
         <v>10</v>
       </c>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
       <c r="AD15" s="9"/>
       <c r="AE15" s="9"/>
       <c r="AF15" s="9"/>
-      <c r="AG15" s="6"/>
-      <c r="AI15" s="5"/>
-      <c r="AJ15" s="6"/>
-      <c r="AL15" s="5"/>
-      <c r="AM15" s="6"/>
-      <c r="AO15" s="5">
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="6"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="6"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="6"/>
+      <c r="AS15" s="5">
         <v>10</v>
       </c>
-      <c r="AP15" s="9"/>
-      <c r="AQ15" s="9"/>
-      <c r="AR15" s="9"/>
-      <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
-      <c r="AU15" s="6"/>
-      <c r="AW15" s="5">
+      <c r="AU15" s="9"/>
+      <c r="AV15" s="9"/>
+      <c r="AW15" s="9"/>
+      <c r="AX15" s="9"/>
+      <c r="AY15" s="26"/>
+      <c r="BB15" s="5">
         <v>10</v>
       </c>
-      <c r="AX15" s="9"/>
-      <c r="AY15" s="9"/>
-      <c r="AZ15" s="9"/>
-      <c r="BA15" s="9"/>
-      <c r="BB15" s="6"/>
-      <c r="BD15" s="5">
-        <v>10</v>
-      </c>
+      <c r="BC15" s="9"/>
+      <c r="BD15" s="9"/>
       <c r="BE15" s="9"/>
-      <c r="BF15" s="11"/>
+      <c r="BF15" s="9"/>
       <c r="BG15" s="9"/>
       <c r="BH15" s="6"/>
-      <c r="BJ15" s="5"/>
-      <c r="BK15" s="6"/>
-      <c r="BM15" s="5"/>
-      <c r="BN15" s="9"/>
-      <c r="BO15" s="9"/>
-      <c r="BP15" s="9"/>
-      <c r="BQ15" s="9"/>
-      <c r="BR15" s="9"/>
-      <c r="BS15" s="6"/>
+      <c r="BJ15" s="5">
+        <v>10</v>
+      </c>
+      <c r="BK15" s="9"/>
+      <c r="BL15" s="11"/>
+      <c r="BM15" s="9"/>
+      <c r="BN15" s="6"/>
+      <c r="BP15" s="5"/>
+      <c r="BQ15" s="6"/>
+      <c r="BS15" s="5"/>
+      <c r="BT15" s="9"/>
+      <c r="BU15" s="9"/>
+      <c r="BV15" s="9"/>
+      <c r="BW15" s="9"/>
+      <c r="BX15" s="9"/>
+      <c r="BY15" s="6"/>
     </row>
-    <row r="16" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AI16" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="BM3:BS3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="AW3:BB3"/>
-    <mergeCell ref="BD3:BH3"/>
-    <mergeCell ref="AO3:AU3"/>
-    <mergeCell ref="BJ3:BK3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Y3:AG3"/>
+  <mergeCells count="14">
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="BS3:BY3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="BB3:BH3"/>
+    <mergeCell ref="BJ3:BN3"/>
+    <mergeCell ref="AS3:AY3"/>
+    <mergeCell ref="BP3:BQ3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AC3:AK3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AR5" r:id="rId1"/>
-    <hyperlink ref="AR6" r:id="rId2"/>
+    <hyperlink ref="AW5" r:id="rId1"/>
+    <hyperlink ref="AW6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Altered SQL scripts to meet new table guidlines
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="111">
   <si>
     <t>fries</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>phone</t>
+  </si>
+  <si>
+    <t>item_type</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -602,6 +605,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,10 +633,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -907,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BY16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AW22" sqref="AW22"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,6 +930,8 @@
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
@@ -967,97 +978,97 @@
       <c r="A3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
-      <c r="L3" s="18" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+      <c r="L3" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="O3" s="21" t="s">
+      <c r="M3" s="26"/>
+      <c r="O3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="23"/>
-      <c r="R3" s="18" t="s">
+      <c r="P3" s="29"/>
+      <c r="R3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="S3" s="20"/>
-      <c r="U3" s="18" t="s">
+      <c r="S3" s="26"/>
+      <c r="U3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="20"/>
-      <c r="Z3" s="18" t="s">
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="26"/>
+      <c r="Z3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AA3" s="20"/>
-      <c r="AC3" s="18" t="s">
+      <c r="AA3" s="26"/>
+      <c r="AC3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="19"/>
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="20"/>
-      <c r="AM3" s="21" t="s">
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
+      <c r="AI3" s="25"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="26"/>
+      <c r="AM3" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="AN3" s="23"/>
-      <c r="AP3" s="21" t="s">
+      <c r="AN3" s="29"/>
+      <c r="AP3" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="AQ3" s="23"/>
-      <c r="AS3" s="18" t="s">
+      <c r="AQ3" s="29"/>
+      <c r="AS3" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AT3" s="19"/>
-      <c r="AU3" s="19"/>
-      <c r="AV3" s="19"/>
-      <c r="AW3" s="19"/>
-      <c r="AX3" s="19"/>
-      <c r="AY3" s="19"/>
-      <c r="BB3" s="18" t="s">
+      <c r="AT3" s="25"/>
+      <c r="AU3" s="25"/>
+      <c r="AV3" s="25"/>
+      <c r="AW3" s="25"/>
+      <c r="AX3" s="25"/>
+      <c r="AY3" s="25"/>
+      <c r="BB3" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="BC3" s="19"/>
-      <c r="BD3" s="19"/>
-      <c r="BE3" s="19"/>
-      <c r="BF3" s="19"/>
-      <c r="BG3" s="19"/>
-      <c r="BH3" s="20"/>
-      <c r="BJ3" s="18" t="s">
+      <c r="BC3" s="25"/>
+      <c r="BD3" s="25"/>
+      <c r="BE3" s="25"/>
+      <c r="BF3" s="25"/>
+      <c r="BG3" s="25"/>
+      <c r="BH3" s="26"/>
+      <c r="BJ3" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="BK3" s="19"/>
-      <c r="BL3" s="19"/>
-      <c r="BM3" s="19"/>
-      <c r="BN3" s="20"/>
-      <c r="BP3" s="18" t="s">
+      <c r="BK3" s="25"/>
+      <c r="BL3" s="25"/>
+      <c r="BM3" s="25"/>
+      <c r="BN3" s="26"/>
+      <c r="BP3" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="BQ3" s="20"/>
-      <c r="BS3" s="21" t="s">
+      <c r="BQ3" s="26"/>
+      <c r="BS3" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="BT3" s="22"/>
-      <c r="BU3" s="22"/>
-      <c r="BV3" s="22"/>
-      <c r="BW3" s="22"/>
-      <c r="BX3" s="22"/>
-      <c r="BY3" s="23"/>
+      <c r="BT3" s="28"/>
+      <c r="BU3" s="28"/>
+      <c r="BV3" s="28"/>
+      <c r="BW3" s="28"/>
+      <c r="BX3" s="28"/>
+      <c r="BY3" s="29"/>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1085,11 +1096,11 @@
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>104</v>
+      <c r="L4" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>40</v>
@@ -1178,7 +1189,7 @@
       <c r="AX4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AY4" s="24" t="s">
+      <c r="AY4" s="20" t="s">
         <v>78</v>
       </c>
       <c r="BB4" s="1" t="s">
@@ -1263,11 +1274,11 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>105</v>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
@@ -1334,7 +1345,7 @@
         <v>12</v>
       </c>
       <c r="AX5" s="7"/>
-      <c r="AY5" s="25">
+      <c r="AY5" s="21">
         <v>1</v>
       </c>
       <c r="BB5" s="3">
@@ -1398,10 +1409,10 @@
       <c r="I6" s="7"/>
       <c r="J6" s="4"/>
       <c r="L6" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="4"/>
@@ -1460,7 +1471,7 @@
         <v>16</v>
       </c>
       <c r="AX6" s="7"/>
-      <c r="AY6" s="25">
+      <c r="AY6" s="21">
         <v>0</v>
       </c>
       <c r="BB6" s="3">
@@ -1522,10 +1533,10 @@
       <c r="I7" s="7"/>
       <c r="J7" s="4"/>
       <c r="L7" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
@@ -1578,7 +1589,7 @@
       <c r="AV7" s="7"/>
       <c r="AW7" s="7"/>
       <c r="AX7" s="7"/>
-      <c r="AY7" s="25"/>
+      <c r="AY7" s="21"/>
       <c r="BB7" s="3">
         <v>2</v>
       </c>
@@ -1635,8 +1646,12 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="4"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4"/>
+      <c r="L8" s="3">
+        <v>3</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
       <c r="R8" s="3">
@@ -1684,11 +1699,11 @@
       <c r="AV8" s="7"/>
       <c r="AW8" s="7"/>
       <c r="AX8" s="7"/>
-      <c r="AY8" s="25"/>
+      <c r="AY8" s="21"/>
       <c r="BB8" s="3">
         <v>3</v>
       </c>
-      <c r="BC8" s="27">
+      <c r="BC8" s="23">
         <v>1</v>
       </c>
       <c r="BD8" s="7"/>
@@ -1774,7 +1789,7 @@
       <c r="AV9" s="7"/>
       <c r="AW9" s="7"/>
       <c r="AX9" s="7"/>
-      <c r="AY9" s="25"/>
+      <c r="AY9" s="21"/>
       <c r="BB9" s="3">
         <v>4</v>
       </c>
@@ -1856,7 +1871,7 @@
       <c r="AV10" s="7"/>
       <c r="AW10" s="7"/>
       <c r="AX10" s="7"/>
-      <c r="AY10" s="25"/>
+      <c r="AY10" s="21"/>
       <c r="BB10" s="3">
         <v>5</v>
       </c>
@@ -1938,7 +1953,7 @@
       <c r="AV11" s="7"/>
       <c r="AW11" s="7"/>
       <c r="AX11" s="7"/>
-      <c r="AY11" s="25"/>
+      <c r="AY11" s="21"/>
       <c r="BB11" s="3">
         <v>6</v>
       </c>
@@ -2016,7 +2031,7 @@
       <c r="AV12" s="7"/>
       <c r="AW12" s="7"/>
       <c r="AX12" s="7"/>
-      <c r="AY12" s="25"/>
+      <c r="AY12" s="21"/>
       <c r="BB12" s="3">
         <v>7</v>
       </c>
@@ -2092,7 +2107,7 @@
       <c r="AV13" s="7"/>
       <c r="AW13" s="7"/>
       <c r="AX13" s="7"/>
-      <c r="AY13" s="25"/>
+      <c r="AY13" s="21"/>
       <c r="BB13" s="3">
         <v>8</v>
       </c>
@@ -2168,7 +2183,7 @@
       <c r="AV14" s="7"/>
       <c r="AW14" s="7"/>
       <c r="AX14" s="7"/>
-      <c r="AY14" s="25"/>
+      <c r="AY14" s="21"/>
       <c r="BB14" s="3">
         <v>9</v>
       </c>
@@ -2209,8 +2224,8 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="6"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="6"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="R15" s="5"/>
@@ -2244,7 +2259,7 @@
       <c r="AV15" s="9"/>
       <c r="AW15" s="9"/>
       <c r="AX15" s="9"/>
-      <c r="AY15" s="26"/>
+      <c r="AY15" s="22"/>
       <c r="BB15" s="5">
         <v>10</v>
       </c>
@@ -2275,6 +2290,8 @@
       <c r="A16" s="17" t="s">
         <v>33</v>
       </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
       <c r="AI16" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Altered scripts to reflect changes to table definitions
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
   <si>
     <t>fries</t>
   </si>
@@ -173,12 +173,6 @@
     <t>discount_percentage</t>
   </si>
   <si>
-    <t>combos</t>
-  </si>
-  <si>
-    <t>combo_id</t>
-  </si>
-  <si>
     <t>time_slots</t>
   </si>
   <si>
@@ -347,9 +341,6 @@
     <t>entrée</t>
   </si>
   <si>
-    <t>combo</t>
-  </si>
-  <si>
     <t>User_id</t>
   </si>
   <si>
@@ -357,6 +348,9 @@
   </si>
   <si>
     <t>item_type</t>
+  </si>
+  <si>
+    <t>package</t>
   </si>
 </sst>
 </file>
@@ -605,16 +599,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -914,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BY16"/>
+  <dimension ref="A2:BV16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,48 +927,46 @@
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="11" customWidth="1"/>
-    <col min="49" max="49" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="11" customWidth="1"/>
+    <col min="46" max="46" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>30</v>
       </c>
@@ -989,7 +981,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="26"/>
       <c r="L3" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M3" s="26"/>
       <c r="O3" s="27" t="s">
@@ -999,76 +991,72 @@
       <c r="R3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="S3" s="26"/>
-      <c r="U3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="26"/>
+      <c r="W3" s="24" t="s">
+        <v>54</v>
+      </c>
       <c r="X3" s="26"/>
       <c r="Z3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="AA3" s="26"/>
-      <c r="AC3" s="24" t="s">
-        <v>58</v>
-      </c>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
       <c r="AD3" s="25"/>
       <c r="AE3" s="25"/>
       <c r="AF3" s="25"/>
       <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="26"/>
+      <c r="AH3" s="26"/>
+      <c r="AJ3" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK3" s="29"/>
       <c r="AM3" s="27" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="AN3" s="29"/>
-      <c r="AP3" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ3" s="29"/>
-      <c r="AS3" s="24" t="s">
-        <v>69</v>
-      </c>
+      <c r="AP3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ3" s="25"/>
+      <c r="AR3" s="25"/>
+      <c r="AS3" s="25"/>
       <c r="AT3" s="25"/>
       <c r="AU3" s="25"/>
       <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="25"/>
-      <c r="BB3" s="24" t="s">
-        <v>80</v>
-      </c>
+      <c r="AY3" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ3" s="25"/>
+      <c r="BA3" s="25"/>
+      <c r="BB3" s="25"/>
       <c r="BC3" s="25"/>
       <c r="BD3" s="25"/>
-      <c r="BE3" s="25"/>
-      <c r="BF3" s="25"/>
-      <c r="BG3" s="25"/>
-      <c r="BH3" s="26"/>
-      <c r="BJ3" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="BK3" s="25"/>
-      <c r="BL3" s="25"/>
-      <c r="BM3" s="25"/>
+      <c r="BE3" s="26"/>
+      <c r="BG3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="BH3" s="25"/>
+      <c r="BI3" s="25"/>
+      <c r="BJ3" s="25"/>
+      <c r="BK3" s="26"/>
+      <c r="BM3" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="BN3" s="26"/>
-      <c r="BP3" s="24" t="s">
+      <c r="BP3" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="BQ3" s="26"/>
-      <c r="BS3" s="27" t="s">
-        <v>94</v>
-      </c>
+      <c r="BQ3" s="28"/>
+      <c r="BR3" s="28"/>
+      <c r="BS3" s="28"/>
       <c r="BT3" s="28"/>
       <c r="BU3" s="28"/>
-      <c r="BV3" s="28"/>
-      <c r="BW3" s="28"/>
-      <c r="BX3" s="28"/>
-      <c r="BY3" s="29"/>
+      <c r="BV3" s="29"/>
     </row>
-    <row r="4" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1070,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>44</v>
@@ -1096,11 +1084,11 @@
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>110</v>
+      <c r="L4" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>40</v>
@@ -1109,34 +1097,37 @@
         <v>48</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="U4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="X4" s="2" t="s">
+      <c r="Z4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>57</v>
+      <c r="AB4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="AD4" s="8" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="AE4" s="8" t="s">
         <v>60</v>
@@ -1145,118 +1136,109 @@
         <v>61</v>
       </c>
       <c r="AG4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AI4" s="8" t="s">
+      <c r="AH4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AJ4" s="8" t="s">
-        <v>64</v>
+      <c r="AJ4" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="1" t="s">
-        <v>59</v>
+      <c r="AR4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS4" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="AT4" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AU4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AV4" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AW4" s="8" t="s">
+      <c r="AV4" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="AX4" s="8" t="s">
+      <c r="AY4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AY4" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="BB4" s="1" t="s">
-        <v>79</v>
+      <c r="AZ4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB4" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="BC4" s="8" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="BD4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="BE4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BF4" s="8" t="s">
+      <c r="BE4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BG4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="BH4" s="2" t="s">
+      <c r="BG4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BJ4" s="1" t="s">
+      <c r="BH4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="BJ4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="BK4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="BL4" s="8" t="s">
+      <c r="BK4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="BM4" s="8" t="s">
-        <v>90</v>
+      <c r="BM4" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="BN4" s="2" t="s">
         <v>91</v>
       </c>
       <c r="BP4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BQ4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BQ4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="BS4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BT4" s="8" t="s">
-        <v>81</v>
+      <c r="BS4" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="BT4" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="BU4" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="BV4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="BW4" s="14" t="s">
+      <c r="BV4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="BX4" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="BY4" s="2" t="s">
-        <v>99</v>
-      </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>39</v>
       </c>
@@ -1274,123 +1256,117 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="4"/>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>104</v>
+      <c r="M5" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
       <c r="R5" s="3">
-        <v>4</v>
-      </c>
-      <c r="S5" s="4">
-        <v>1</v>
-      </c>
-      <c r="U5" s="3">
         <v>0</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="W5" s="7" t="s">
+      <c r="T5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="U5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="W5" s="3">
+        <v>2</v>
+      </c>
+      <c r="X5" s="4">
+        <v>3</v>
+      </c>
       <c r="Z5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="4">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="3">
         <v>0</v>
       </c>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
+      <c r="AF5" s="7">
+        <v>1</v>
+      </c>
       <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AJ5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="AM5" s="3">
         <v>0</v>
       </c>
       <c r="AN5" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="AP5" s="3">
         <v>0</v>
       </c>
-      <c r="AQ5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="AS5" s="3">
+      <c r="AQ5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS5" s="7"/>
+      <c r="AT5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="19">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="3">
         <v>0</v>
       </c>
-      <c r="AT5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="AU5" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV5" s="7"/>
-      <c r="AW5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="AX5" s="7"/>
-      <c r="AY5" s="21">
+      <c r="AZ5" s="7">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="7"/>
+      <c r="BB5" s="7"/>
+      <c r="BC5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="BD5" s="7"/>
+      <c r="BE5" s="4"/>
+      <c r="BG5" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="7">
         <v>1</v>
       </c>
-      <c r="BB5" s="3">
+      <c r="BI5" s="10">
+        <v>554466778899</v>
+      </c>
+      <c r="BJ5" s="12">
+        <v>43718</v>
+      </c>
+      <c r="BK5" s="4">
+        <v>234</v>
+      </c>
+      <c r="BM5" s="3">
         <v>0</v>
       </c>
-      <c r="BC5" s="7">
-        <v>0</v>
-      </c>
-      <c r="BD5" s="7"/>
-      <c r="BE5" s="7"/>
-      <c r="BF5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="BG5" s="7"/>
-      <c r="BH5" s="4"/>
-      <c r="BJ5" s="3">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="7">
-        <v>1</v>
-      </c>
-      <c r="BL5" s="10">
-        <v>554466778899</v>
-      </c>
-      <c r="BM5" s="12">
-        <v>43718</v>
-      </c>
-      <c r="BN5" s="4">
-        <v>234</v>
-      </c>
-      <c r="BP5" s="3">
-        <v>0</v>
-      </c>
-      <c r="BQ5" s="4" t="s">
+      <c r="BN5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="BS5" s="3"/>
+      <c r="BP5" s="3"/>
+      <c r="BQ5" s="7"/>
+      <c r="BR5" s="7"/>
+      <c r="BS5" s="7"/>
       <c r="BT5" s="7"/>
       <c r="BU5" s="7"/>
-      <c r="BV5" s="7"/>
-      <c r="BW5" s="7"/>
-      <c r="BX5" s="7"/>
-      <c r="BY5" s="4"/>
+      <c r="BV5" s="4"/>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
@@ -1412,109 +1388,103 @@
         <v>1</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="4"/>
       <c r="R6" s="3">
+        <v>1</v>
+      </c>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="4"/>
+      <c r="W6" s="3">
+        <v>2</v>
+      </c>
+      <c r="X6" s="4">
         <v>4</v>
       </c>
-      <c r="S6" s="4">
-        <v>2</v>
-      </c>
-      <c r="U6" s="3">
+      <c r="Z6" s="3">
         <v>1</v>
       </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="4"/>
-      <c r="Z6" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="4">
-        <v>4</v>
-      </c>
-      <c r="AC6" s="3">
-        <v>1</v>
-      </c>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
       <c r="AG6" s="7"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7"/>
-      <c r="AJ6" s="7"/>
-      <c r="AK6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AJ6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="AM6" s="3">
         <v>1</v>
       </c>
       <c r="AN6" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AP6" s="3">
         <v>1</v>
       </c>
-      <c r="AQ6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS6" s="3">
+      <c r="AQ6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS6" s="7"/>
+      <c r="AT6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU6" s="7"/>
+      <c r="AV6" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="3">
         <v>1</v>
       </c>
-      <c r="AT6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="AV6" s="7"/>
-      <c r="AW6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX6" s="7"/>
-      <c r="AY6" s="21">
+      <c r="AZ6" s="7">
         <v>0</v>
       </c>
-      <c r="BB6" s="3">
+      <c r="BA6" s="7"/>
+      <c r="BB6" s="7"/>
+      <c r="BC6" s="7"/>
+      <c r="BD6" s="7"/>
+      <c r="BE6" s="4"/>
+      <c r="BG6" s="3">
         <v>1</v>
       </c>
-      <c r="BC6" s="7">
-        <v>0</v>
-      </c>
-      <c r="BD6" s="7"/>
-      <c r="BE6" s="7"/>
-      <c r="BF6" s="7"/>
-      <c r="BG6" s="7"/>
-      <c r="BH6" s="4"/>
-      <c r="BJ6" s="3">
+      <c r="BH6" s="7">
         <v>1</v>
       </c>
-      <c r="BK6" s="7">
+      <c r="BI6" s="10">
+        <v>683967034588</v>
+      </c>
+      <c r="BJ6" s="12">
+        <v>43957</v>
+      </c>
+      <c r="BK6" s="4">
+        <v>354</v>
+      </c>
+      <c r="BM6" s="3">
         <v>1</v>
       </c>
-      <c r="BL6" s="10">
-        <v>683967034588</v>
-      </c>
-      <c r="BM6" s="12">
-        <v>43957</v>
-      </c>
-      <c r="BN6" s="4">
-        <v>354</v>
-      </c>
-      <c r="BP6" s="3">
-        <v>1</v>
-      </c>
-      <c r="BQ6" s="4" t="s">
+      <c r="BN6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="BS6" s="3"/>
+      <c r="BP6" s="3"/>
+      <c r="BQ6" s="7"/>
+      <c r="BR6" s="7"/>
+      <c r="BS6" s="7"/>
       <c r="BT6" s="7"/>
       <c r="BU6" s="7"/>
-      <c r="BV6" s="7"/>
-      <c r="BW6" s="7"/>
-      <c r="BX6" s="7"/>
-      <c r="BY6" s="4"/>
+      <c r="BV6" s="4"/>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>18</v>
       </c>
@@ -1536,101 +1506,95 @@
         <v>2</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
       <c r="R7" s="3">
-        <v>4</v>
-      </c>
-      <c r="S7" s="4">
-        <v>3</v>
-      </c>
-      <c r="U7" s="3">
         <v>2</v>
       </c>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="4"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="4"/>
+      <c r="W7" s="3">
+        <v>2</v>
+      </c>
+      <c r="X7" s="4">
+        <v>5</v>
+      </c>
       <c r="Z7" s="3">
         <v>2</v>
       </c>
-      <c r="AA7" s="4">
-        <v>5</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>2</v>
-      </c>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="7"/>
       <c r="AG7" s="7"/>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="7"/>
-      <c r="AK7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AJ7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="AM7" s="3">
         <v>2</v>
       </c>
       <c r="AN7" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="AP7" s="3">
         <v>2</v>
       </c>
-      <c r="AQ7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AS7" s="3">
-        <v>2</v>
-      </c>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="7"/>
       <c r="AT7" s="7"/>
       <c r="AU7" s="7"/>
-      <c r="AV7" s="7"/>
-      <c r="AW7" s="7"/>
-      <c r="AX7" s="7"/>
-      <c r="AY7" s="21"/>
-      <c r="BB7" s="3">
+      <c r="AV7" s="19"/>
+      <c r="AY7" s="3">
         <v>2</v>
       </c>
-      <c r="BC7" s="7">
+      <c r="AZ7" s="7">
         <v>1</v>
       </c>
+      <c r="BA7" s="7"/>
+      <c r="BB7" s="7"/>
+      <c r="BC7" s="7"/>
       <c r="BD7" s="7"/>
-      <c r="BE7" s="7"/>
-      <c r="BF7" s="7"/>
-      <c r="BG7" s="7"/>
-      <c r="BH7" s="4"/>
-      <c r="BJ7" s="3">
+      <c r="BE7" s="4"/>
+      <c r="BG7" s="3">
         <v>2</v>
       </c>
-      <c r="BK7" s="7">
+      <c r="BH7" s="7">
         <v>2</v>
       </c>
-      <c r="BL7" s="10">
+      <c r="BI7" s="10">
         <v>338744976569</v>
       </c>
-      <c r="BM7" s="12">
+      <c r="BJ7" s="12">
         <v>45770</v>
       </c>
-      <c r="BN7" s="4">
+      <c r="BK7" s="4">
         <v>325</v>
       </c>
-      <c r="BP7" s="3">
+      <c r="BM7" s="3">
         <v>2</v>
       </c>
-      <c r="BQ7" s="4" t="s">
+      <c r="BN7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="BS7" s="3"/>
+      <c r="BP7" s="3"/>
+      <c r="BQ7" s="7"/>
+      <c r="BR7" s="7"/>
+      <c r="BS7" s="7"/>
       <c r="BT7" s="7"/>
       <c r="BU7" s="7"/>
-      <c r="BV7" s="7"/>
-      <c r="BW7" s="7"/>
-      <c r="BX7" s="7"/>
-      <c r="BY7" s="4"/>
+      <c r="BV7" s="4"/>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
@@ -1650,89 +1614,83 @@
         <v>3</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
       <c r="R8" s="3">
-        <v>5</v>
-      </c>
-      <c r="S8" s="4">
+        <v>3</v>
+      </c>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="4"/>
+      <c r="W8" s="3">
+        <v>2</v>
+      </c>
+      <c r="X8" s="4">
         <v>1</v>
       </c>
-      <c r="U8" s="3">
+      <c r="Z8" s="3">
         <v>3</v>
       </c>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="4"/>
-      <c r="Z8" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="3">
-        <v>3</v>
-      </c>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
       <c r="AF8" s="7"/>
       <c r="AG8" s="7"/>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="7"/>
-      <c r="AJ8" s="7"/>
-      <c r="AK8" s="4"/>
-      <c r="AM8" s="3">
+      <c r="AH8" s="4"/>
+      <c r="AJ8" s="3">
         <v>3</v>
       </c>
-      <c r="AN8" s="4" t="s">
+      <c r="AK8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AP8" s="3"/>
-      <c r="AQ8" s="4"/>
-      <c r="AS8" s="3">
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="4"/>
+      <c r="AP8" s="3">
         <v>3</v>
       </c>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
       <c r="AT8" s="7"/>
       <c r="AU8" s="7"/>
-      <c r="AV8" s="7"/>
-      <c r="AW8" s="7"/>
-      <c r="AX8" s="7"/>
-      <c r="AY8" s="21"/>
-      <c r="BB8" s="3">
+      <c r="AV8" s="19"/>
+      <c r="AY8" s="3">
         <v>3</v>
       </c>
-      <c r="BC8" s="23">
+      <c r="AZ8" s="21">
         <v>1</v>
       </c>
+      <c r="BA8" s="7"/>
+      <c r="BB8" s="7"/>
+      <c r="BC8" s="7"/>
       <c r="BD8" s="7"/>
-      <c r="BE8" s="7"/>
-      <c r="BF8" s="7"/>
-      <c r="BG8" s="7"/>
-      <c r="BH8" s="4"/>
-      <c r="BJ8" s="3">
+      <c r="BE8" s="4"/>
+      <c r="BG8" s="3">
         <v>3</v>
       </c>
-      <c r="BK8" s="7"/>
-      <c r="BL8" s="10"/>
-      <c r="BM8" s="7"/>
-      <c r="BN8" s="4"/>
-      <c r="BP8" s="3">
+      <c r="BH8" s="7"/>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="7"/>
+      <c r="BK8" s="4"/>
+      <c r="BM8" s="3">
         <v>3</v>
       </c>
-      <c r="BQ8" s="4" t="s">
+      <c r="BN8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="BS8" s="3"/>
+      <c r="BP8" s="3"/>
+      <c r="BQ8" s="7"/>
+      <c r="BR8" s="7"/>
+      <c r="BS8" s="7"/>
       <c r="BT8" s="7"/>
       <c r="BU8" s="7"/>
-      <c r="BV8" s="7"/>
-      <c r="BW8" s="7"/>
-      <c r="BX8" s="7"/>
-      <c r="BY8" s="4"/>
+      <c r="BV8" s="4"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
@@ -1753,74 +1711,68 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
       <c r="R9" s="3">
-        <v>5</v>
-      </c>
-      <c r="S9" s="4">
         <v>4</v>
       </c>
-      <c r="U9" s="3">
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="4"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="4"/>
+      <c r="Z9" s="3">
         <v>4</v>
       </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="4"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="4"/>
-      <c r="AC9" s="3">
-        <v>4</v>
-      </c>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
       <c r="AG9" s="7"/>
-      <c r="AH9" s="7"/>
-      <c r="AI9" s="7"/>
-      <c r="AJ9" s="7"/>
+      <c r="AH9" s="4"/>
+      <c r="AJ9" s="3"/>
       <c r="AK9" s="4"/>
       <c r="AM9" s="3"/>
       <c r="AN9" s="4"/>
-      <c r="AP9" s="3"/>
-      <c r="AQ9" s="4"/>
-      <c r="AS9" s="3">
+      <c r="AP9" s="3">
         <v>4</v>
       </c>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="7"/>
       <c r="AT9" s="7"/>
       <c r="AU9" s="7"/>
-      <c r="AV9" s="7"/>
-      <c r="AW9" s="7"/>
-      <c r="AX9" s="7"/>
-      <c r="AY9" s="21"/>
-      <c r="BB9" s="3">
+      <c r="AV9" s="19"/>
+      <c r="AY9" s="3">
         <v>4</v>
       </c>
+      <c r="AZ9" s="7"/>
+      <c r="BA9" s="7"/>
+      <c r="BB9" s="7"/>
       <c r="BC9" s="7"/>
       <c r="BD9" s="7"/>
-      <c r="BE9" s="7"/>
-      <c r="BF9" s="7"/>
-      <c r="BG9" s="7"/>
-      <c r="BH9" s="4"/>
-      <c r="BJ9" s="3">
+      <c r="BE9" s="4"/>
+      <c r="BG9" s="3">
         <v>4</v>
       </c>
-      <c r="BK9" s="7"/>
-      <c r="BL9" s="10"/>
-      <c r="BM9" s="7"/>
-      <c r="BN9" s="4"/>
-      <c r="BP9" s="3">
+      <c r="BH9" s="7"/>
+      <c r="BI9" s="10"/>
+      <c r="BJ9" s="7"/>
+      <c r="BK9" s="4"/>
+      <c r="BM9" s="3">
         <v>4</v>
       </c>
-      <c r="BQ9" s="4" t="s">
+      <c r="BN9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="BS9" s="3"/>
+      <c r="BP9" s="3"/>
+      <c r="BQ9" s="7"/>
+      <c r="BR9" s="7"/>
+      <c r="BS9" s="7"/>
       <c r="BT9" s="7"/>
       <c r="BU9" s="7"/>
-      <c r="BV9" s="7"/>
-      <c r="BW9" s="7"/>
-      <c r="BX9" s="7"/>
-      <c r="BY9" s="4"/>
+      <c r="BV9" s="4"/>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>26</v>
       </c>
@@ -1838,71 +1790,69 @@
       <c r="M10" s="4"/>
       <c r="O10" s="3"/>
       <c r="P10" s="4"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="4"/>
-      <c r="U10" s="3">
+      <c r="R10" s="3">
         <v>5</v>
       </c>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="4"/>
+      <c r="W10" s="3"/>
       <c r="X10" s="4"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="4"/>
-      <c r="AC10" s="3">
+      <c r="Z10" s="3">
         <v>5</v>
       </c>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
       <c r="AE10" s="7"/>
       <c r="AF10" s="7"/>
       <c r="AG10" s="7"/>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="7"/>
-      <c r="AJ10" s="7"/>
+      <c r="AH10" s="4"/>
+      <c r="AJ10" s="3"/>
       <c r="AK10" s="4"/>
       <c r="AM10" s="3"/>
       <c r="AN10" s="4"/>
-      <c r="AP10" s="3"/>
-      <c r="AQ10" s="4"/>
-      <c r="AS10" s="3">
+      <c r="AP10" s="3">
         <v>5</v>
       </c>
+      <c r="AQ10" s="7"/>
+      <c r="AR10" s="7"/>
+      <c r="AS10" s="7"/>
       <c r="AT10" s="7"/>
       <c r="AU10" s="7"/>
-      <c r="AV10" s="7"/>
-      <c r="AW10" s="7"/>
-      <c r="AX10" s="7"/>
-      <c r="AY10" s="21"/>
-      <c r="BB10" s="3">
+      <c r="AV10" s="19"/>
+      <c r="AY10" s="3">
         <v>5</v>
       </c>
+      <c r="AZ10" s="7"/>
+      <c r="BA10" s="7"/>
+      <c r="BB10" s="7"/>
       <c r="BC10" s="7"/>
       <c r="BD10" s="7"/>
-      <c r="BE10" s="7"/>
-      <c r="BF10" s="7"/>
-      <c r="BG10" s="7"/>
-      <c r="BH10" s="4"/>
-      <c r="BJ10" s="3">
+      <c r="BE10" s="4"/>
+      <c r="BG10" s="3">
         <v>5</v>
       </c>
-      <c r="BK10" s="7"/>
-      <c r="BL10" s="10"/>
-      <c r="BM10" s="7"/>
-      <c r="BN10" s="4"/>
-      <c r="BP10" s="3">
+      <c r="BH10" s="7"/>
+      <c r="BI10" s="10"/>
+      <c r="BJ10" s="7"/>
+      <c r="BK10" s="4"/>
+      <c r="BM10" s="3">
         <v>5</v>
       </c>
-      <c r="BQ10" s="4" t="s">
+      <c r="BN10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="BS10" s="3"/>
+      <c r="BP10" s="3"/>
+      <c r="BQ10" s="7"/>
+      <c r="BR10" s="7"/>
+      <c r="BS10" s="7"/>
       <c r="BT10" s="7"/>
       <c r="BU10" s="7"/>
-      <c r="BV10" s="7"/>
-      <c r="BW10" s="7"/>
-      <c r="BX10" s="7"/>
-      <c r="BY10" s="4"/>
+      <c r="BV10" s="4"/>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>38</v>
       </c>
@@ -1920,67 +1870,65 @@
       <c r="M11" s="4"/>
       <c r="O11" s="3"/>
       <c r="P11" s="4"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="4"/>
-      <c r="U11" s="3">
+      <c r="R11" s="3">
         <v>6</v>
       </c>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="4"/>
+      <c r="W11" s="3"/>
       <c r="X11" s="4"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="4"/>
-      <c r="AC11" s="3">
+      <c r="Z11" s="3">
         <v>6</v>
       </c>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
       <c r="AE11" s="7"/>
       <c r="AF11" s="7"/>
       <c r="AG11" s="7"/>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="7"/>
-      <c r="AJ11" s="7"/>
+      <c r="AH11" s="4"/>
+      <c r="AJ11" s="3"/>
       <c r="AK11" s="4"/>
       <c r="AM11" s="3"/>
       <c r="AN11" s="4"/>
-      <c r="AP11" s="3"/>
-      <c r="AQ11" s="4"/>
-      <c r="AS11" s="3">
+      <c r="AP11" s="3">
         <v>6</v>
       </c>
+      <c r="AQ11" s="7"/>
+      <c r="AR11" s="7"/>
+      <c r="AS11" s="7"/>
       <c r="AT11" s="7"/>
       <c r="AU11" s="7"/>
-      <c r="AV11" s="7"/>
-      <c r="AW11" s="7"/>
-      <c r="AX11" s="7"/>
-      <c r="AY11" s="21"/>
-      <c r="BB11" s="3">
+      <c r="AV11" s="19"/>
+      <c r="AY11" s="3">
         <v>6</v>
       </c>
+      <c r="AZ11" s="7"/>
+      <c r="BA11" s="7"/>
+      <c r="BB11" s="7"/>
       <c r="BC11" s="7"/>
       <c r="BD11" s="7"/>
-      <c r="BE11" s="7"/>
-      <c r="BF11" s="7"/>
-      <c r="BG11" s="7"/>
-      <c r="BH11" s="4"/>
-      <c r="BJ11" s="3">
+      <c r="BE11" s="4"/>
+      <c r="BG11" s="3">
         <v>6</v>
       </c>
-      <c r="BK11" s="7"/>
-      <c r="BL11" s="10"/>
-      <c r="BM11" s="7"/>
+      <c r="BH11" s="7"/>
+      <c r="BI11" s="10"/>
+      <c r="BJ11" s="7"/>
+      <c r="BK11" s="4"/>
+      <c r="BM11" s="3"/>
       <c r="BN11" s="4"/>
       <c r="BP11" s="3"/>
-      <c r="BQ11" s="4"/>
-      <c r="BS11" s="3"/>
+      <c r="BQ11" s="7"/>
+      <c r="BR11" s="7"/>
+      <c r="BS11" s="7"/>
       <c r="BT11" s="7"/>
       <c r="BU11" s="7"/>
-      <c r="BV11" s="7"/>
-      <c r="BW11" s="7"/>
-      <c r="BX11" s="7"/>
-      <c r="BY11" s="4"/>
+      <c r="BV11" s="4"/>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
@@ -1998,67 +1946,65 @@
       <c r="M12" s="4"/>
       <c r="O12" s="3"/>
       <c r="P12" s="4"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="4"/>
-      <c r="U12" s="3">
+      <c r="R12" s="3">
         <v>7</v>
       </c>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="4"/>
+      <c r="W12" s="3"/>
       <c r="X12" s="4"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="4"/>
-      <c r="AC12" s="3">
+      <c r="Z12" s="3">
         <v>7</v>
       </c>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
-      <c r="AH12" s="7"/>
-      <c r="AI12" s="7"/>
-      <c r="AJ12" s="7"/>
+      <c r="AH12" s="4"/>
+      <c r="AJ12" s="3"/>
       <c r="AK12" s="4"/>
       <c r="AM12" s="3"/>
       <c r="AN12" s="4"/>
-      <c r="AP12" s="3"/>
-      <c r="AQ12" s="4"/>
-      <c r="AS12" s="3">
+      <c r="AP12" s="3">
         <v>7</v>
       </c>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="7"/>
+      <c r="AS12" s="7"/>
       <c r="AT12" s="7"/>
       <c r="AU12" s="7"/>
-      <c r="AV12" s="7"/>
-      <c r="AW12" s="7"/>
-      <c r="AX12" s="7"/>
-      <c r="AY12" s="21"/>
-      <c r="BB12" s="3">
+      <c r="AV12" s="19"/>
+      <c r="AY12" s="3">
         <v>7</v>
       </c>
+      <c r="AZ12" s="7"/>
+      <c r="BA12" s="7"/>
+      <c r="BB12" s="7"/>
       <c r="BC12" s="7"/>
       <c r="BD12" s="7"/>
-      <c r="BE12" s="7"/>
-      <c r="BF12" s="7"/>
-      <c r="BG12" s="7"/>
-      <c r="BH12" s="4"/>
-      <c r="BJ12" s="3">
+      <c r="BE12" s="4"/>
+      <c r="BG12" s="3">
         <v>7</v>
       </c>
-      <c r="BK12" s="7"/>
-      <c r="BL12" s="10"/>
-      <c r="BM12" s="7"/>
+      <c r="BH12" s="7"/>
+      <c r="BI12" s="10"/>
+      <c r="BJ12" s="7"/>
+      <c r="BK12" s="4"/>
+      <c r="BM12" s="3"/>
       <c r="BN12" s="4"/>
       <c r="BP12" s="3"/>
-      <c r="BQ12" s="4"/>
-      <c r="BS12" s="3"/>
+      <c r="BQ12" s="7"/>
+      <c r="BR12" s="7"/>
+      <c r="BS12" s="7"/>
       <c r="BT12" s="7"/>
       <c r="BU12" s="7"/>
-      <c r="BV12" s="7"/>
-      <c r="BW12" s="7"/>
-      <c r="BX12" s="7"/>
-      <c r="BY12" s="4"/>
+      <c r="BV12" s="4"/>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>8</v>
       </c>
@@ -2077,64 +2023,62 @@
       <c r="O13" s="3"/>
       <c r="P13" s="4"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="4"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="4"/>
+      <c r="W13" s="3"/>
       <c r="X13" s="4"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="4"/>
-      <c r="AC13" s="3">
+      <c r="Z13" s="3">
         <v>8</v>
       </c>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
       <c r="AE13" s="7"/>
       <c r="AF13" s="7"/>
       <c r="AG13" s="7"/>
-      <c r="AH13" s="7"/>
-      <c r="AI13" s="7"/>
-      <c r="AJ13" s="7"/>
+      <c r="AH13" s="4"/>
+      <c r="AJ13" s="3"/>
       <c r="AK13" s="4"/>
       <c r="AM13" s="3"/>
       <c r="AN13" s="4"/>
-      <c r="AP13" s="3"/>
-      <c r="AQ13" s="4"/>
-      <c r="AS13" s="3">
+      <c r="AP13" s="3">
         <v>8</v>
       </c>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="7"/>
+      <c r="AS13" s="7"/>
       <c r="AT13" s="7"/>
       <c r="AU13" s="7"/>
-      <c r="AV13" s="7"/>
-      <c r="AW13" s="7"/>
-      <c r="AX13" s="7"/>
-      <c r="AY13" s="21"/>
-      <c r="BB13" s="3">
+      <c r="AV13" s="19"/>
+      <c r="AY13" s="3">
         <v>8</v>
       </c>
+      <c r="AZ13" s="7"/>
+      <c r="BA13" s="7"/>
+      <c r="BB13" s="7"/>
       <c r="BC13" s="7"/>
       <c r="BD13" s="7"/>
-      <c r="BE13" s="7"/>
-      <c r="BF13" s="7"/>
-      <c r="BG13" s="7"/>
-      <c r="BH13" s="4"/>
-      <c r="BJ13" s="3">
+      <c r="BE13" s="4"/>
+      <c r="BG13" s="3">
         <v>8</v>
       </c>
-      <c r="BK13" s="7"/>
-      <c r="BL13" s="10"/>
-      <c r="BM13" s="7"/>
+      <c r="BH13" s="7"/>
+      <c r="BI13" s="10"/>
+      <c r="BJ13" s="7"/>
+      <c r="BK13" s="4"/>
+      <c r="BM13" s="3"/>
       <c r="BN13" s="4"/>
       <c r="BP13" s="3"/>
-      <c r="BQ13" s="4"/>
-      <c r="BS13" s="3"/>
+      <c r="BQ13" s="7"/>
+      <c r="BR13" s="7"/>
+      <c r="BS13" s="7"/>
       <c r="BT13" s="7"/>
       <c r="BU13" s="7"/>
-      <c r="BV13" s="7"/>
-      <c r="BW13" s="7"/>
-      <c r="BX13" s="7"/>
-      <c r="BY13" s="4"/>
+      <c r="BV13" s="4"/>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>32</v>
       </c>
@@ -2153,64 +2097,62 @@
       <c r="O14" s="3"/>
       <c r="P14" s="4"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="4"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="4"/>
+      <c r="W14" s="3"/>
       <c r="X14" s="4"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="4"/>
-      <c r="AC14" s="3">
+      <c r="Z14" s="3">
         <v>9</v>
       </c>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
       <c r="AF14" s="7"/>
       <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
+      <c r="AH14" s="4"/>
+      <c r="AJ14" s="3"/>
       <c r="AK14" s="4"/>
       <c r="AM14" s="3"/>
       <c r="AN14" s="4"/>
-      <c r="AP14" s="3"/>
-      <c r="AQ14" s="4"/>
-      <c r="AS14" s="3">
+      <c r="AP14" s="3">
         <v>9</v>
       </c>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="7"/>
+      <c r="AS14" s="7"/>
       <c r="AT14" s="7"/>
       <c r="AU14" s="7"/>
-      <c r="AV14" s="7"/>
-      <c r="AW14" s="7"/>
-      <c r="AX14" s="7"/>
-      <c r="AY14" s="21"/>
-      <c r="BB14" s="3">
+      <c r="AV14" s="19"/>
+      <c r="AY14" s="3">
         <v>9</v>
       </c>
+      <c r="AZ14" s="7"/>
+      <c r="BA14" s="7"/>
+      <c r="BB14" s="7"/>
       <c r="BC14" s="7"/>
       <c r="BD14" s="7"/>
-      <c r="BE14" s="7"/>
-      <c r="BF14" s="7"/>
-      <c r="BG14" s="7"/>
-      <c r="BH14" s="4"/>
-      <c r="BJ14" s="3">
+      <c r="BE14" s="4"/>
+      <c r="BG14" s="3">
         <v>9</v>
       </c>
-      <c r="BK14" s="7"/>
-      <c r="BL14" s="10"/>
-      <c r="BM14" s="7"/>
+      <c r="BH14" s="7"/>
+      <c r="BI14" s="10"/>
+      <c r="BJ14" s="7"/>
+      <c r="BK14" s="4"/>
+      <c r="BM14" s="3"/>
       <c r="BN14" s="4"/>
       <c r="BP14" s="3"/>
-      <c r="BQ14" s="4"/>
-      <c r="BS14" s="3"/>
+      <c r="BQ14" s="7"/>
+      <c r="BR14" s="7"/>
+      <c r="BS14" s="7"/>
       <c r="BT14" s="7"/>
       <c r="BU14" s="7"/>
-      <c r="BV14" s="7"/>
-      <c r="BW14" s="7"/>
-      <c r="BX14" s="7"/>
-      <c r="BY14" s="4"/>
+      <c r="BV14" s="4"/>
     </row>
-    <row r="15" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>25</v>
       </c>
@@ -2224,98 +2166,95 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="6"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="6"/>
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="R15" s="5"/>
-      <c r="S15" s="6"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="6"/>
+      <c r="W15" s="5"/>
       <c r="X15" s="6"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="6"/>
-      <c r="AC15" s="5">
+      <c r="Z15" s="5">
         <v>10</v>
       </c>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
       <c r="AD15" s="9"/>
       <c r="AE15" s="9"/>
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
+      <c r="AH15" s="6"/>
+      <c r="AJ15" s="5"/>
       <c r="AK15" s="6"/>
       <c r="AM15" s="5"/>
       <c r="AN15" s="6"/>
-      <c r="AP15" s="5"/>
-      <c r="AQ15" s="6"/>
-      <c r="AS15" s="5">
+      <c r="AP15" s="5">
         <v>10</v>
       </c>
+      <c r="AQ15" s="9"/>
+      <c r="AR15" s="9"/>
+      <c r="AS15" s="9"/>
       <c r="AT15" s="9"/>
       <c r="AU15" s="9"/>
-      <c r="AV15" s="9"/>
-      <c r="AW15" s="9"/>
-      <c r="AX15" s="9"/>
-      <c r="AY15" s="22"/>
-      <c r="BB15" s="5">
+      <c r="AV15" s="20"/>
+      <c r="AY15" s="5">
         <v>10</v>
       </c>
+      <c r="AZ15" s="9"/>
+      <c r="BA15" s="9"/>
+      <c r="BB15" s="9"/>
       <c r="BC15" s="9"/>
       <c r="BD15" s="9"/>
-      <c r="BE15" s="9"/>
-      <c r="BF15" s="9"/>
-      <c r="BG15" s="9"/>
-      <c r="BH15" s="6"/>
-      <c r="BJ15" s="5">
+      <c r="BE15" s="6"/>
+      <c r="BG15" s="5">
         <v>10</v>
       </c>
-      <c r="BK15" s="9"/>
-      <c r="BL15" s="11"/>
-      <c r="BM15" s="9"/>
+      <c r="BH15" s="9"/>
+      <c r="BI15" s="11"/>
+      <c r="BJ15" s="9"/>
+      <c r="BK15" s="6"/>
+      <c r="BM15" s="5"/>
       <c r="BN15" s="6"/>
       <c r="BP15" s="5"/>
-      <c r="BQ15" s="6"/>
-      <c r="BS15" s="5"/>
+      <c r="BQ15" s="9"/>
+      <c r="BR15" s="9"/>
+      <c r="BS15" s="9"/>
       <c r="BT15" s="9"/>
       <c r="BU15" s="9"/>
-      <c r="BV15" s="9"/>
-      <c r="BW15" s="9"/>
-      <c r="BX15" s="9"/>
-      <c r="BY15" s="6"/>
+      <c r="BV15" s="6"/>
     </row>
-    <row r="16" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
-      <c r="AI16" t="s">
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="AF16" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="C3:J3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="BS3:BY3"/>
-    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="BP3:BV3"/>
     <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="AJ3:AK3"/>
     <mergeCell ref="O3:P3"/>
-    <mergeCell ref="U3:X3"/>
-    <mergeCell ref="BB3:BH3"/>
-    <mergeCell ref="BJ3:BN3"/>
-    <mergeCell ref="AS3:AY3"/>
-    <mergeCell ref="BP3:BQ3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AC3:AK3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="AY3:BE3"/>
+    <mergeCell ref="BG3:BK3"/>
+    <mergeCell ref="AP3:AV3"/>
+    <mergeCell ref="BM3:BN3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z3:AH3"/>
     <mergeCell ref="L3:M3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AW5" r:id="rId1"/>
-    <hyperlink ref="AW6" r:id="rId2"/>
+    <hyperlink ref="AT5" r:id="rId1"/>
+    <hyperlink ref="AT6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>